<commit_message>
Manage import and update the liste of the logements
</commit_message>
<xml_diff>
--- a/static/files/logements.xlsx
+++ b/static/files/logements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasoudard/workspace/beta.gouv.fr/appel/static/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C73FC2A6-8AFE-DE45-AADA-207F973A7C73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{523498FE-E506-4140-94ED-1F95835DE110}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31060" yWindow="3060" windowWidth="27020" windowHeight="16440" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Ici quelques explications</t>
   </si>
@@ -56,24 +56,12 @@
     <t>Attention, en aucun cas vous ne devez modifier l'entête du tableau des prêts, cela casserait l'import des données</t>
   </si>
   <si>
-    <t>Désignation</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
-    <t>Surface habitable</t>
-  </si>
-  <si>
-    <t>Loyer maxinum en € par m2 de surface utile</t>
-  </si>
-  <si>
     <t>Coefficient propre au logement</t>
   </si>
   <si>
-    <t>Loyer maxinum du logement en €</t>
-  </si>
-  <si>
     <t>Type de logement</t>
   </si>
   <si>
@@ -92,26 +80,64 @@
     <t>T5 et plus</t>
   </si>
   <si>
-    <t>Surface des annexes réelle</t>
-  </si>
-  <si>
-    <t>Surface utile</t>
-  </si>
-  <si>
     <t>si des logements sont déjà assignés à la convention, alors ils seront exportés dans le fichier modèle</t>
   </si>
   <si>
     <t>5. Vérifier le contenu téléversé dans l'application et enrigistrer en cliquant sur le bouton 'Enregistrer et Suivant'</t>
   </si>
   <si>
-    <t>Surface des annexes retenue dans la SU</t>
+    <t>Col 1</t>
+  </si>
+  <si>
+    <t>Col 2</t>
+  </si>
+  <si>
+    <t>Col 3</t>
+  </si>
+  <si>
+    <t>Col 4</t>
+  </si>
+  <si>
+    <t>Col 5</t>
+  </si>
+  <si>
+    <t>Col 6</t>
+  </si>
+  <si>
+    <t>Col 7</t>
+  </si>
+  <si>
+    <t>Désignation des logements</t>
+  </si>
+  <si>
+    <t>Surface utile
+(surface habitable augmentée de 50% de la surface des annexes)</t>
+  </si>
+  <si>
+    <t>Surface des annexes
+Retenue dans la SU</t>
+  </si>
+  <si>
+    <t>Surface des annexes
+Réelle</t>
+  </si>
+  <si>
+    <t>Surface habitable
+(article R.111-2)</t>
+  </si>
+  <si>
+    <t>Loyer maxinum en € par m² de surface utile</t>
+  </si>
+  <si>
+    <t>Loyer maxinum du logement en €
+(col 4 * col 5 * col 6)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -140,8 +166,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -154,8 +188,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -192,26 +232,123 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="5">
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
@@ -280,31 +417,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -319,24 +431,6 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CE610699-E1F9-0A4E-92A0-C2463FA7C402}" name="Table2" displayName="Table2" ref="A1:I51" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:I51" xr:uid="{CE610699-E1F9-0A4E-92A0-C2463FA7C402}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{C27C0725-DFC5-8941-AA1D-4AA3540CBB4A}" name="Désignation"/>
-    <tableColumn id="2" xr3:uid="{82FED836-92E4-D94B-95D2-D5F3693D5EB9}" name="Type"/>
-    <tableColumn id="3" xr3:uid="{EC09CAB2-EF86-6D49-BC29-EA9B1F4DA654}" name="Surface habitable"/>
-    <tableColumn id="4" xr3:uid="{6DE00705-339F-A245-8F5C-197410239E91}" name="Surface des annexes réelle"/>
-    <tableColumn id="6" xr3:uid="{1A2E2C82-EEBA-2440-A5FD-437DE359B24F}" name="Surface des annexes retenue dans la SU"/>
-    <tableColumn id="5" xr3:uid="{DBC9DD41-246B-3B4B-A5DC-0E0BB51834D7}" name="Surface utile"/>
-    <tableColumn id="9" xr3:uid="{7980F62E-959D-FC4E-BFF0-EA96FE743DCC}" name="Loyer maxinum en € par m2 de surface utile"/>
-    <tableColumn id="10" xr3:uid="{56DC6C49-6BF0-6D4E-B703-4009F2A3F997}" name="Coefficient propre au logement"/>
-    <tableColumn id="11" xr3:uid="{9B17FE5D-6DE8-DD44-9315-CDB91C2D1223}" name="Loyer maxinum du logement en €"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{60458129-C213-8741-80B4-B15A740996D3}" name="type" displayName="type" ref="A1:A6" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3" tableBorderDxfId="2" totalsRowBorderDxfId="1">
   <autoFilter ref="A1:A6" xr:uid="{60458129-C213-8741-80B4-B15A740996D3}"/>
   <tableColumns count="1">
@@ -643,10 +737,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08021C90-1ACF-2A4C-A1B0-58A48A8F7007}">
-  <dimension ref="A1:Q7"/>
+  <dimension ref="A1:Q51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -654,63 +748,622 @@
     <col min="1" max="9" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="34" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:17" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="I1" s="24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="21"/>
+      <c r="C2" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E2" s="21"/>
+      <c r="F2" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>11</v>
-      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A3" s="13"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="15"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4" s="10"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="12"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5" s="13"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="15"/>
     </row>
     <row r="6" spans="1:17" ht="20" x14ac:dyDescent="0.2">
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="7"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
     </row>
     <row r="7" spans="1:17" ht="20" x14ac:dyDescent="0.2">
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
+      <c r="A7" s="13"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8" s="10"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="12"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9" s="13"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="15"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A10" s="10"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="12"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A11" s="13"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="15"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A12" s="10"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="12"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A13" s="13"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="15"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A14" s="10"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="12"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A15" s="13"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="15"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A16" s="10"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="12"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="13"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="15"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="10"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="12"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="13"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="15"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="10"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="12"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="13"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="15"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="10"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="12"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="13"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="15"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="10"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="12"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="13"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="15"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="10"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="12"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="13"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="15"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="10"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="12"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="13"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="15"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="10"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="12"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="13"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="15"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="10"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="12"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" s="13"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="14"/>
+      <c r="I33" s="15"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" s="10"/>
+      <c r="B34" s="11"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="12"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" s="13"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="14"/>
+      <c r="I35" s="15"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" s="10"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="11"/>
+      <c r="I36" s="12"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" s="13"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="14"/>
+      <c r="I37" s="15"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38" s="10"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="11"/>
+      <c r="I38" s="12"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39" s="13"/>
+      <c r="B39" s="14"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="14"/>
+      <c r="G39" s="14"/>
+      <c r="H39" s="14"/>
+      <c r="I39" s="15"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A40" s="10"/>
+      <c r="B40" s="11"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="11"/>
+      <c r="H40" s="11"/>
+      <c r="I40" s="12"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" s="13"/>
+      <c r="B41" s="14"/>
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="14"/>
+      <c r="I41" s="15"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A42" s="10"/>
+      <c r="B42" s="11"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="11"/>
+      <c r="H42" s="11"/>
+      <c r="I42" s="12"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43" s="13"/>
+      <c r="B43" s="14"/>
+      <c r="C43" s="14"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="14"/>
+      <c r="H43" s="14"/>
+      <c r="I43" s="15"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A44" s="10"/>
+      <c r="B44" s="11"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="11"/>
+      <c r="G44" s="11"/>
+      <c r="H44" s="11"/>
+      <c r="I44" s="12"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A45" s="13"/>
+      <c r="B45" s="14"/>
+      <c r="C45" s="14"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="14"/>
+      <c r="G45" s="14"/>
+      <c r="H45" s="14"/>
+      <c r="I45" s="15"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A46" s="10"/>
+      <c r="B46" s="11"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="11"/>
+      <c r="F46" s="11"/>
+      <c r="G46" s="11"/>
+      <c r="H46" s="11"/>
+      <c r="I46" s="12"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A47" s="13"/>
+      <c r="B47" s="14"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="14"/>
+      <c r="G47" s="14"/>
+      <c r="H47" s="14"/>
+      <c r="I47" s="15"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A48" s="10"/>
+      <c r="B48" s="11"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="11"/>
+      <c r="F48" s="11"/>
+      <c r="G48" s="11"/>
+      <c r="H48" s="11"/>
+      <c r="I48" s="12"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A49" s="13"/>
+      <c r="B49" s="14"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
+      <c r="H49" s="14"/>
+      <c r="I49" s="15"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A50" s="10"/>
+      <c r="B50" s="11"/>
+      <c r="C50" s="11"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="11"/>
+      <c r="F50" s="11"/>
+      <c r="G50" s="11"/>
+      <c r="H50" s="11"/>
+      <c r="I50" s="12"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A51" s="7"/>
+      <c r="B51" s="8"/>
+      <c r="C51" s="8"/>
+      <c r="D51" s="8"/>
+      <c r="E51" s="8"/>
+      <c r="F51" s="8"/>
+      <c r="G51" s="8"/>
+      <c r="H51" s="8"/>
+      <c r="I51" s="9"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:E2"/>
+  </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -718,7 +1371,7 @@
           <x14:formula1>
             <xm:f>Data!$A$2:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B51</xm:sqref>
+          <xm:sqref>B3:B51</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -752,7 +1405,7 @@
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.2">
@@ -772,7 +1425,7 @@
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.2">
@@ -798,37 +1451,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
+      <c r="A7" s="4"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="IA/ID92IMnFhCvhdUjY4hoG+EPrNrHjo/Xj8oRPxM3icZk1457m9NYmxClUCr+lzs5b3p2NBiV3MdwIquvHA8g==" saltValue="Kw8wu+/yu2vZV8ifFGisyw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>

</xml_diff>

<commit_message>
Manage import and update the liste of the logements (#25)
</commit_message>
<xml_diff>
--- a/static/files/logements.xlsx
+++ b/static/files/logements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasoudard/workspace/beta.gouv.fr/appel/static/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C73FC2A6-8AFE-DE45-AADA-207F973A7C73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{523498FE-E506-4140-94ED-1F95835DE110}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31060" yWindow="3060" windowWidth="27020" windowHeight="16440" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Ici quelques explications</t>
   </si>
@@ -56,24 +56,12 @@
     <t>Attention, en aucun cas vous ne devez modifier l'entête du tableau des prêts, cela casserait l'import des données</t>
   </si>
   <si>
-    <t>Désignation</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
-    <t>Surface habitable</t>
-  </si>
-  <si>
-    <t>Loyer maxinum en € par m2 de surface utile</t>
-  </si>
-  <si>
     <t>Coefficient propre au logement</t>
   </si>
   <si>
-    <t>Loyer maxinum du logement en €</t>
-  </si>
-  <si>
     <t>Type de logement</t>
   </si>
   <si>
@@ -92,26 +80,64 @@
     <t>T5 et plus</t>
   </si>
   <si>
-    <t>Surface des annexes réelle</t>
-  </si>
-  <si>
-    <t>Surface utile</t>
-  </si>
-  <si>
     <t>si des logements sont déjà assignés à la convention, alors ils seront exportés dans le fichier modèle</t>
   </si>
   <si>
     <t>5. Vérifier le contenu téléversé dans l'application et enrigistrer en cliquant sur le bouton 'Enregistrer et Suivant'</t>
   </si>
   <si>
-    <t>Surface des annexes retenue dans la SU</t>
+    <t>Col 1</t>
+  </si>
+  <si>
+    <t>Col 2</t>
+  </si>
+  <si>
+    <t>Col 3</t>
+  </si>
+  <si>
+    <t>Col 4</t>
+  </si>
+  <si>
+    <t>Col 5</t>
+  </si>
+  <si>
+    <t>Col 6</t>
+  </si>
+  <si>
+    <t>Col 7</t>
+  </si>
+  <si>
+    <t>Désignation des logements</t>
+  </si>
+  <si>
+    <t>Surface utile
+(surface habitable augmentée de 50% de la surface des annexes)</t>
+  </si>
+  <si>
+    <t>Surface des annexes
+Retenue dans la SU</t>
+  </si>
+  <si>
+    <t>Surface des annexes
+Réelle</t>
+  </si>
+  <si>
+    <t>Surface habitable
+(article R.111-2)</t>
+  </si>
+  <si>
+    <t>Loyer maxinum en € par m² de surface utile</t>
+  </si>
+  <si>
+    <t>Loyer maxinum du logement en €
+(col 4 * col 5 * col 6)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -140,8 +166,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -154,8 +188,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -192,26 +232,123 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="5">
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
@@ -280,31 +417,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -319,24 +431,6 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CE610699-E1F9-0A4E-92A0-C2463FA7C402}" name="Table2" displayName="Table2" ref="A1:I51" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:I51" xr:uid="{CE610699-E1F9-0A4E-92A0-C2463FA7C402}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{C27C0725-DFC5-8941-AA1D-4AA3540CBB4A}" name="Désignation"/>
-    <tableColumn id="2" xr3:uid="{82FED836-92E4-D94B-95D2-D5F3693D5EB9}" name="Type"/>
-    <tableColumn id="3" xr3:uid="{EC09CAB2-EF86-6D49-BC29-EA9B1F4DA654}" name="Surface habitable"/>
-    <tableColumn id="4" xr3:uid="{6DE00705-339F-A245-8F5C-197410239E91}" name="Surface des annexes réelle"/>
-    <tableColumn id="6" xr3:uid="{1A2E2C82-EEBA-2440-A5FD-437DE359B24F}" name="Surface des annexes retenue dans la SU"/>
-    <tableColumn id="5" xr3:uid="{DBC9DD41-246B-3B4B-A5DC-0E0BB51834D7}" name="Surface utile"/>
-    <tableColumn id="9" xr3:uid="{7980F62E-959D-FC4E-BFF0-EA96FE743DCC}" name="Loyer maxinum en € par m2 de surface utile"/>
-    <tableColumn id="10" xr3:uid="{56DC6C49-6BF0-6D4E-B703-4009F2A3F997}" name="Coefficient propre au logement"/>
-    <tableColumn id="11" xr3:uid="{9B17FE5D-6DE8-DD44-9315-CDB91C2D1223}" name="Loyer maxinum du logement en €"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{60458129-C213-8741-80B4-B15A740996D3}" name="type" displayName="type" ref="A1:A6" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3" tableBorderDxfId="2" totalsRowBorderDxfId="1">
   <autoFilter ref="A1:A6" xr:uid="{60458129-C213-8741-80B4-B15A740996D3}"/>
   <tableColumns count="1">
@@ -643,10 +737,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08021C90-1ACF-2A4C-A1B0-58A48A8F7007}">
-  <dimension ref="A1:Q7"/>
+  <dimension ref="A1:Q51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -654,63 +748,622 @@
     <col min="1" max="9" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="34" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:17" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="I1" s="24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="21"/>
+      <c r="C2" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E2" s="21"/>
+      <c r="F2" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>11</v>
-      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A3" s="13"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="15"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4" s="10"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="12"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5" s="13"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="15"/>
     </row>
     <row r="6" spans="1:17" ht="20" x14ac:dyDescent="0.2">
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="7"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
     </row>
     <row r="7" spans="1:17" ht="20" x14ac:dyDescent="0.2">
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
+      <c r="A7" s="13"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8" s="10"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="12"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9" s="13"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="15"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A10" s="10"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="12"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A11" s="13"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="15"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A12" s="10"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="12"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A13" s="13"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="15"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A14" s="10"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="12"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A15" s="13"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="15"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A16" s="10"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="12"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="13"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="15"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="10"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="12"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="13"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="15"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="10"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="12"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="13"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="15"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="10"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="12"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="13"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="15"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="10"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="12"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="13"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="15"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="10"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="12"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="13"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="15"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="10"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="12"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="13"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="15"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="10"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="12"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="13"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="15"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="10"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="12"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" s="13"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="14"/>
+      <c r="I33" s="15"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" s="10"/>
+      <c r="B34" s="11"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="12"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" s="13"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="14"/>
+      <c r="I35" s="15"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" s="10"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="11"/>
+      <c r="I36" s="12"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" s="13"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="14"/>
+      <c r="I37" s="15"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38" s="10"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="11"/>
+      <c r="I38" s="12"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39" s="13"/>
+      <c r="B39" s="14"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="14"/>
+      <c r="G39" s="14"/>
+      <c r="H39" s="14"/>
+      <c r="I39" s="15"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A40" s="10"/>
+      <c r="B40" s="11"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="11"/>
+      <c r="H40" s="11"/>
+      <c r="I40" s="12"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" s="13"/>
+      <c r="B41" s="14"/>
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="14"/>
+      <c r="I41" s="15"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A42" s="10"/>
+      <c r="B42" s="11"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="11"/>
+      <c r="H42" s="11"/>
+      <c r="I42" s="12"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43" s="13"/>
+      <c r="B43" s="14"/>
+      <c r="C43" s="14"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="14"/>
+      <c r="H43" s="14"/>
+      <c r="I43" s="15"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A44" s="10"/>
+      <c r="B44" s="11"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="11"/>
+      <c r="G44" s="11"/>
+      <c r="H44" s="11"/>
+      <c r="I44" s="12"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A45" s="13"/>
+      <c r="B45" s="14"/>
+      <c r="C45" s="14"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="14"/>
+      <c r="G45" s="14"/>
+      <c r="H45" s="14"/>
+      <c r="I45" s="15"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A46" s="10"/>
+      <c r="B46" s="11"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="11"/>
+      <c r="F46" s="11"/>
+      <c r="G46" s="11"/>
+      <c r="H46" s="11"/>
+      <c r="I46" s="12"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A47" s="13"/>
+      <c r="B47" s="14"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="14"/>
+      <c r="G47" s="14"/>
+      <c r="H47" s="14"/>
+      <c r="I47" s="15"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A48" s="10"/>
+      <c r="B48" s="11"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="11"/>
+      <c r="F48" s="11"/>
+      <c r="G48" s="11"/>
+      <c r="H48" s="11"/>
+      <c r="I48" s="12"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A49" s="13"/>
+      <c r="B49" s="14"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
+      <c r="H49" s="14"/>
+      <c r="I49" s="15"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A50" s="10"/>
+      <c r="B50" s="11"/>
+      <c r="C50" s="11"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="11"/>
+      <c r="F50" s="11"/>
+      <c r="G50" s="11"/>
+      <c r="H50" s="11"/>
+      <c r="I50" s="12"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A51" s="7"/>
+      <c r="B51" s="8"/>
+      <c r="C51" s="8"/>
+      <c r="D51" s="8"/>
+      <c r="E51" s="8"/>
+      <c r="F51" s="8"/>
+      <c r="G51" s="8"/>
+      <c r="H51" s="8"/>
+      <c r="I51" s="9"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:E2"/>
+  </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -718,7 +1371,7 @@
           <x14:formula1>
             <xm:f>Data!$A$2:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B51</xm:sqref>
+          <xm:sqref>B3:B51</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -752,7 +1405,7 @@
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.2">
@@ -772,7 +1425,7 @@
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.2">
@@ -798,37 +1451,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
+      <c r="A7" s="4"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="IA/ID92IMnFhCvhdUjY4hoG+EPrNrHjo/Xj8oRPxM3icZk1457m9NYmxClUCr+lzs5b3p2NBiV3MdwIquvHA8g==" saltValue="Kw8wu+/yu2vZV8ifFGisyw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>

</xml_diff>

<commit_message>
Manage Import Export and save
</commit_message>
<xml_diff>
--- a/static/files/logements.xlsx
+++ b/static/files/logements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasoudard/workspace/beta.gouv.fr/appel/static/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{523498FE-E506-4140-94ED-1F95835DE110}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC952250-F910-1D4D-BBFC-39F10E6DECCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31060" yWindow="3060" windowWidth="27020" windowHeight="16440" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
@@ -137,6 +137,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="#,##0.00\ [$€-40C]"/>
+    <numFmt numFmtId="165" formatCode="#,##0.000"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -304,7 +308,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -314,25 +318,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -344,6 +337,26 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -749,102 +762,102 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="84" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="G1" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="I1" s="17" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="18" t="s">
+      <c r="B2" s="19"/>
+      <c r="C2" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="21"/>
-      <c r="F2" s="18" t="s">
+      <c r="E2" s="19"/>
+      <c r="F2" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="19" t="s">
+      <c r="I2" s="14" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A3" s="13"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="15"/>
+      <c r="A3" s="11"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="26"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4" s="10"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="12"/>
+      <c r="A4" s="9"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="27"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5" s="13"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="15"/>
+      <c r="A5" s="11"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="26"/>
     </row>
     <row r="6" spans="1:17" ht="20" x14ac:dyDescent="0.2">
-      <c r="A6" s="10"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="16"/>
+      <c r="A6" s="9"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="28"/>
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
       <c r="L6" s="5"/>
@@ -855,15 +868,15 @@
       <c r="Q6" s="6"/>
     </row>
     <row r="7" spans="1:17" ht="20" x14ac:dyDescent="0.2">
-      <c r="A7" s="13"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="17"/>
+      <c r="A7" s="11"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="29"/>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
       <c r="L7" s="5"/>
@@ -874,488 +887,488 @@
       <c r="Q7" s="6"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A8" s="10"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="12"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="27"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A9" s="13"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="15"/>
+      <c r="A9" s="11"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="26"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A10" s="10"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="12"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="27"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A11" s="13"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="15"/>
+      <c r="A11" s="11"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="26"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A12" s="10"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="12"/>
+      <c r="A12" s="9"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="27"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A13" s="13"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="15"/>
+      <c r="A13" s="11"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="26"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A14" s="10"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="12"/>
+      <c r="A14" s="9"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="27"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A15" s="13"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="15"/>
+      <c r="A15" s="11"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="26"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A16" s="10"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="12"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="27"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="13"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="15"/>
+      <c r="A17" s="11"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="31"/>
+      <c r="I17" s="26"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="10"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="12"/>
+      <c r="A18" s="9"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="27"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="13"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="15"/>
+      <c r="A19" s="11"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="31"/>
+      <c r="I19" s="26"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="10"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="12"/>
+      <c r="A20" s="9"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="27"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="13"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="15"/>
+      <c r="A21" s="11"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="31"/>
+      <c r="I21" s="26"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="10"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="12"/>
+      <c r="A22" s="9"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="32"/>
+      <c r="I22" s="27"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="13"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="15"/>
+      <c r="A23" s="11"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="31"/>
+      <c r="I23" s="26"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="10"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="12"/>
+      <c r="A24" s="9"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="27"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="13"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="15"/>
+      <c r="A25" s="11"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="31"/>
+      <c r="I25" s="26"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="10"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="12"/>
+      <c r="A26" s="9"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="32"/>
+      <c r="I26" s="27"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="13"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="15"/>
+      <c r="A27" s="11"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="26"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="10"/>
-      <c r="B28" s="11"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="12"/>
+      <c r="A28" s="9"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="27"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="13"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="15"/>
+      <c r="A29" s="11"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="31"/>
+      <c r="I29" s="26"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="10"/>
-      <c r="B30" s="11"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="12"/>
+      <c r="A30" s="9"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="32"/>
+      <c r="I30" s="27"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" s="13"/>
-      <c r="B31" s="14"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="14"/>
-      <c r="I31" s="15"/>
+      <c r="A31" s="11"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="23"/>
+      <c r="H31" s="31"/>
+      <c r="I31" s="26"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" s="10"/>
-      <c r="B32" s="11"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="11"/>
-      <c r="I32" s="12"/>
+      <c r="A32" s="9"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="24"/>
+      <c r="H32" s="32"/>
+      <c r="I32" s="27"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" s="13"/>
-      <c r="B33" s="14"/>
-      <c r="C33" s="14"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
-      <c r="I33" s="15"/>
+      <c r="A33" s="11"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="23"/>
+      <c r="H33" s="31"/>
+      <c r="I33" s="26"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="10"/>
-      <c r="B34" s="11"/>
-      <c r="C34" s="11"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="11"/>
-      <c r="I34" s="12"/>
+      <c r="A34" s="9"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="24"/>
+      <c r="H34" s="32"/>
+      <c r="I34" s="27"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" s="13"/>
-      <c r="B35" s="14"/>
-      <c r="C35" s="14"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="14"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="14"/>
-      <c r="I35" s="15"/>
+      <c r="A35" s="11"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="23"/>
+      <c r="H35" s="31"/>
+      <c r="I35" s="26"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" s="10"/>
-      <c r="B36" s="11"/>
-      <c r="C36" s="11"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="11"/>
-      <c r="F36" s="11"/>
-      <c r="G36" s="11"/>
-      <c r="H36" s="11"/>
-      <c r="I36" s="12"/>
+      <c r="A36" s="9"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="24"/>
+      <c r="H36" s="32"/>
+      <c r="I36" s="27"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" s="13"/>
-      <c r="B37" s="14"/>
-      <c r="C37" s="14"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="14"/>
-      <c r="F37" s="14"/>
-      <c r="G37" s="14"/>
-      <c r="H37" s="14"/>
-      <c r="I37" s="15"/>
+      <c r="A37" s="11"/>
+      <c r="B37" s="12"/>
+      <c r="C37" s="20"/>
+      <c r="D37" s="20"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="20"/>
+      <c r="G37" s="23"/>
+      <c r="H37" s="31"/>
+      <c r="I37" s="26"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A38" s="10"/>
-      <c r="B38" s="11"/>
-      <c r="C38" s="11"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="11"/>
-      <c r="F38" s="11"/>
-      <c r="G38" s="11"/>
-      <c r="H38" s="11"/>
-      <c r="I38" s="12"/>
+      <c r="A38" s="9"/>
+      <c r="B38" s="10"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="24"/>
+      <c r="H38" s="32"/>
+      <c r="I38" s="27"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A39" s="13"/>
-      <c r="B39" s="14"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="14"/>
-      <c r="G39" s="14"/>
-      <c r="H39" s="14"/>
-      <c r="I39" s="15"/>
+      <c r="A39" s="11"/>
+      <c r="B39" s="12"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="20"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="20"/>
+      <c r="G39" s="23"/>
+      <c r="H39" s="31"/>
+      <c r="I39" s="26"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A40" s="10"/>
-      <c r="B40" s="11"/>
-      <c r="C40" s="11"/>
-      <c r="D40" s="11"/>
-      <c r="E40" s="11"/>
-      <c r="F40" s="11"/>
-      <c r="G40" s="11"/>
-      <c r="H40" s="11"/>
-      <c r="I40" s="12"/>
+      <c r="A40" s="9"/>
+      <c r="B40" s="10"/>
+      <c r="C40" s="21"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="21"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="24"/>
+      <c r="H40" s="32"/>
+      <c r="I40" s="27"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A41" s="13"/>
-      <c r="B41" s="14"/>
-      <c r="C41" s="14"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="14"/>
-      <c r="G41" s="14"/>
-      <c r="H41" s="14"/>
-      <c r="I41" s="15"/>
+      <c r="A41" s="11"/>
+      <c r="B41" s="12"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="20"/>
+      <c r="G41" s="23"/>
+      <c r="H41" s="31"/>
+      <c r="I41" s="26"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A42" s="10"/>
-      <c r="B42" s="11"/>
-      <c r="C42" s="11"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="11"/>
-      <c r="F42" s="11"/>
-      <c r="G42" s="11"/>
-      <c r="H42" s="11"/>
-      <c r="I42" s="12"/>
+      <c r="A42" s="9"/>
+      <c r="B42" s="10"/>
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21"/>
+      <c r="G42" s="24"/>
+      <c r="H42" s="32"/>
+      <c r="I42" s="27"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A43" s="13"/>
-      <c r="B43" s="14"/>
-      <c r="C43" s="14"/>
-      <c r="D43" s="14"/>
-      <c r="E43" s="14"/>
-      <c r="F43" s="14"/>
-      <c r="G43" s="14"/>
-      <c r="H43" s="14"/>
-      <c r="I43" s="15"/>
+      <c r="A43" s="11"/>
+      <c r="B43" s="12"/>
+      <c r="C43" s="20"/>
+      <c r="D43" s="20"/>
+      <c r="E43" s="20"/>
+      <c r="F43" s="20"/>
+      <c r="G43" s="23"/>
+      <c r="H43" s="31"/>
+      <c r="I43" s="26"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A44" s="10"/>
-      <c r="B44" s="11"/>
-      <c r="C44" s="11"/>
-      <c r="D44" s="11"/>
-      <c r="E44" s="11"/>
-      <c r="F44" s="11"/>
-      <c r="G44" s="11"/>
-      <c r="H44" s="11"/>
-      <c r="I44" s="12"/>
+      <c r="A44" s="9"/>
+      <c r="B44" s="10"/>
+      <c r="C44" s="21"/>
+      <c r="D44" s="21"/>
+      <c r="E44" s="21"/>
+      <c r="F44" s="21"/>
+      <c r="G44" s="24"/>
+      <c r="H44" s="32"/>
+      <c r="I44" s="27"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A45" s="13"/>
-      <c r="B45" s="14"/>
-      <c r="C45" s="14"/>
-      <c r="D45" s="14"/>
-      <c r="E45" s="14"/>
-      <c r="F45" s="14"/>
-      <c r="G45" s="14"/>
-      <c r="H45" s="14"/>
-      <c r="I45" s="15"/>
+      <c r="A45" s="11"/>
+      <c r="B45" s="12"/>
+      <c r="C45" s="20"/>
+      <c r="D45" s="20"/>
+      <c r="E45" s="20"/>
+      <c r="F45" s="20"/>
+      <c r="G45" s="23"/>
+      <c r="H45" s="31"/>
+      <c r="I45" s="26"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A46" s="10"/>
-      <c r="B46" s="11"/>
-      <c r="C46" s="11"/>
-      <c r="D46" s="11"/>
-      <c r="E46" s="11"/>
-      <c r="F46" s="11"/>
-      <c r="G46" s="11"/>
-      <c r="H46" s="11"/>
-      <c r="I46" s="12"/>
+      <c r="A46" s="9"/>
+      <c r="B46" s="10"/>
+      <c r="C46" s="21"/>
+      <c r="D46" s="21"/>
+      <c r="E46" s="21"/>
+      <c r="F46" s="21"/>
+      <c r="G46" s="24"/>
+      <c r="H46" s="32"/>
+      <c r="I46" s="27"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A47" s="13"/>
-      <c r="B47" s="14"/>
-      <c r="C47" s="14"/>
-      <c r="D47" s="14"/>
-      <c r="E47" s="14"/>
-      <c r="F47" s="14"/>
-      <c r="G47" s="14"/>
-      <c r="H47" s="14"/>
-      <c r="I47" s="15"/>
+      <c r="A47" s="11"/>
+      <c r="B47" s="12"/>
+      <c r="C47" s="20"/>
+      <c r="D47" s="20"/>
+      <c r="E47" s="20"/>
+      <c r="F47" s="20"/>
+      <c r="G47" s="23"/>
+      <c r="H47" s="31"/>
+      <c r="I47" s="26"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A48" s="10"/>
-      <c r="B48" s="11"/>
-      <c r="C48" s="11"/>
-      <c r="D48" s="11"/>
-      <c r="E48" s="11"/>
-      <c r="F48" s="11"/>
-      <c r="G48" s="11"/>
-      <c r="H48" s="11"/>
-      <c r="I48" s="12"/>
+      <c r="A48" s="9"/>
+      <c r="B48" s="10"/>
+      <c r="C48" s="21"/>
+      <c r="D48" s="21"/>
+      <c r="E48" s="21"/>
+      <c r="F48" s="21"/>
+      <c r="G48" s="24"/>
+      <c r="H48" s="32"/>
+      <c r="I48" s="27"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A49" s="13"/>
-      <c r="B49" s="14"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
-      <c r="H49" s="14"/>
-      <c r="I49" s="15"/>
+      <c r="A49" s="11"/>
+      <c r="B49" s="12"/>
+      <c r="C49" s="20"/>
+      <c r="D49" s="20"/>
+      <c r="E49" s="20"/>
+      <c r="F49" s="20"/>
+      <c r="G49" s="23"/>
+      <c r="H49" s="31"/>
+      <c r="I49" s="26"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A50" s="10"/>
-      <c r="B50" s="11"/>
-      <c r="C50" s="11"/>
-      <c r="D50" s="11"/>
-      <c r="E50" s="11"/>
-      <c r="F50" s="11"/>
-      <c r="G50" s="11"/>
-      <c r="H50" s="11"/>
-      <c r="I50" s="12"/>
+      <c r="A50" s="9"/>
+      <c r="B50" s="10"/>
+      <c r="C50" s="21"/>
+      <c r="D50" s="21"/>
+      <c r="E50" s="21"/>
+      <c r="F50" s="21"/>
+      <c r="G50" s="24"/>
+      <c r="H50" s="32"/>
+      <c r="I50" s="27"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="7"/>
       <c r="B51" s="8"/>
-      <c r="C51" s="8"/>
-      <c r="D51" s="8"/>
-      <c r="E51" s="8"/>
-      <c r="F51" s="8"/>
-      <c r="G51" s="8"/>
-      <c r="H51" s="8"/>
-      <c r="I51" s="9"/>
+      <c r="C51" s="22"/>
+      <c r="D51" s="22"/>
+      <c r="E51" s="22"/>
+      <c r="F51" s="22"/>
+      <c r="G51" s="25"/>
+      <c r="H51" s="33"/>
+      <c r="I51" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Step7 manage annexes (#27)
* Manage Import Export and save

* manage that the logement of the annexe belongs to the lot : using the designation
</commit_message>
<xml_diff>
--- a/static/files/logements.xlsx
+++ b/static/files/logements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasoudard/workspace/beta.gouv.fr/appel/static/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{523498FE-E506-4140-94ED-1F95835DE110}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC952250-F910-1D4D-BBFC-39F10E6DECCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31060" yWindow="3060" windowWidth="27020" windowHeight="16440" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
@@ -137,6 +137,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="#,##0.00\ [$€-40C]"/>
+    <numFmt numFmtId="165" formatCode="#,##0.000"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -304,7 +308,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -314,25 +318,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -344,6 +337,26 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -749,102 +762,102 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="84" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="G1" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="I1" s="17" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="18" t="s">
+      <c r="B2" s="19"/>
+      <c r="C2" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="21"/>
-      <c r="F2" s="18" t="s">
+      <c r="E2" s="19"/>
+      <c r="F2" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="19" t="s">
+      <c r="I2" s="14" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A3" s="13"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="15"/>
+      <c r="A3" s="11"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="26"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4" s="10"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="12"/>
+      <c r="A4" s="9"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="27"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5" s="13"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="15"/>
+      <c r="A5" s="11"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="26"/>
     </row>
     <row r="6" spans="1:17" ht="20" x14ac:dyDescent="0.2">
-      <c r="A6" s="10"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="16"/>
+      <c r="A6" s="9"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="28"/>
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
       <c r="L6" s="5"/>
@@ -855,15 +868,15 @@
       <c r="Q6" s="6"/>
     </row>
     <row r="7" spans="1:17" ht="20" x14ac:dyDescent="0.2">
-      <c r="A7" s="13"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="17"/>
+      <c r="A7" s="11"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="29"/>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
       <c r="L7" s="5"/>
@@ -874,488 +887,488 @@
       <c r="Q7" s="6"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A8" s="10"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="12"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="27"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A9" s="13"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="15"/>
+      <c r="A9" s="11"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="26"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A10" s="10"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="12"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="27"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A11" s="13"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="15"/>
+      <c r="A11" s="11"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="26"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A12" s="10"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="12"/>
+      <c r="A12" s="9"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="27"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A13" s="13"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="15"/>
+      <c r="A13" s="11"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="26"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A14" s="10"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="12"/>
+      <c r="A14" s="9"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="27"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A15" s="13"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="15"/>
+      <c r="A15" s="11"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="26"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A16" s="10"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="12"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="27"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="13"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="15"/>
+      <c r="A17" s="11"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="31"/>
+      <c r="I17" s="26"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="10"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="12"/>
+      <c r="A18" s="9"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="27"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="13"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="15"/>
+      <c r="A19" s="11"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="31"/>
+      <c r="I19" s="26"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="10"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="12"/>
+      <c r="A20" s="9"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="27"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="13"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="15"/>
+      <c r="A21" s="11"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="31"/>
+      <c r="I21" s="26"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="10"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="12"/>
+      <c r="A22" s="9"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="32"/>
+      <c r="I22" s="27"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="13"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="15"/>
+      <c r="A23" s="11"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="31"/>
+      <c r="I23" s="26"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="10"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="12"/>
+      <c r="A24" s="9"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="27"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="13"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="15"/>
+      <c r="A25" s="11"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="31"/>
+      <c r="I25" s="26"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="10"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="12"/>
+      <c r="A26" s="9"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="32"/>
+      <c r="I26" s="27"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="13"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="15"/>
+      <c r="A27" s="11"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="26"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="10"/>
-      <c r="B28" s="11"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="12"/>
+      <c r="A28" s="9"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="27"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="13"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="15"/>
+      <c r="A29" s="11"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="31"/>
+      <c r="I29" s="26"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="10"/>
-      <c r="B30" s="11"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="12"/>
+      <c r="A30" s="9"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="32"/>
+      <c r="I30" s="27"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" s="13"/>
-      <c r="B31" s="14"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="14"/>
-      <c r="I31" s="15"/>
+      <c r="A31" s="11"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="23"/>
+      <c r="H31" s="31"/>
+      <c r="I31" s="26"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" s="10"/>
-      <c r="B32" s="11"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="11"/>
-      <c r="I32" s="12"/>
+      <c r="A32" s="9"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="24"/>
+      <c r="H32" s="32"/>
+      <c r="I32" s="27"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" s="13"/>
-      <c r="B33" s="14"/>
-      <c r="C33" s="14"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
-      <c r="I33" s="15"/>
+      <c r="A33" s="11"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="23"/>
+      <c r="H33" s="31"/>
+      <c r="I33" s="26"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="10"/>
-      <c r="B34" s="11"/>
-      <c r="C34" s="11"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="11"/>
-      <c r="I34" s="12"/>
+      <c r="A34" s="9"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="24"/>
+      <c r="H34" s="32"/>
+      <c r="I34" s="27"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" s="13"/>
-      <c r="B35" s="14"/>
-      <c r="C35" s="14"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="14"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="14"/>
-      <c r="I35" s="15"/>
+      <c r="A35" s="11"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="23"/>
+      <c r="H35" s="31"/>
+      <c r="I35" s="26"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" s="10"/>
-      <c r="B36" s="11"/>
-      <c r="C36" s="11"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="11"/>
-      <c r="F36" s="11"/>
-      <c r="G36" s="11"/>
-      <c r="H36" s="11"/>
-      <c r="I36" s="12"/>
+      <c r="A36" s="9"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="24"/>
+      <c r="H36" s="32"/>
+      <c r="I36" s="27"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" s="13"/>
-      <c r="B37" s="14"/>
-      <c r="C37" s="14"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="14"/>
-      <c r="F37" s="14"/>
-      <c r="G37" s="14"/>
-      <c r="H37" s="14"/>
-      <c r="I37" s="15"/>
+      <c r="A37" s="11"/>
+      <c r="B37" s="12"/>
+      <c r="C37" s="20"/>
+      <c r="D37" s="20"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="20"/>
+      <c r="G37" s="23"/>
+      <c r="H37" s="31"/>
+      <c r="I37" s="26"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A38" s="10"/>
-      <c r="B38" s="11"/>
-      <c r="C38" s="11"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="11"/>
-      <c r="F38" s="11"/>
-      <c r="G38" s="11"/>
-      <c r="H38" s="11"/>
-      <c r="I38" s="12"/>
+      <c r="A38" s="9"/>
+      <c r="B38" s="10"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="24"/>
+      <c r="H38" s="32"/>
+      <c r="I38" s="27"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A39" s="13"/>
-      <c r="B39" s="14"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="14"/>
-      <c r="G39" s="14"/>
-      <c r="H39" s="14"/>
-      <c r="I39" s="15"/>
+      <c r="A39" s="11"/>
+      <c r="B39" s="12"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="20"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="20"/>
+      <c r="G39" s="23"/>
+      <c r="H39" s="31"/>
+      <c r="I39" s="26"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A40" s="10"/>
-      <c r="B40" s="11"/>
-      <c r="C40" s="11"/>
-      <c r="D40" s="11"/>
-      <c r="E40" s="11"/>
-      <c r="F40" s="11"/>
-      <c r="G40" s="11"/>
-      <c r="H40" s="11"/>
-      <c r="I40" s="12"/>
+      <c r="A40" s="9"/>
+      <c r="B40" s="10"/>
+      <c r="C40" s="21"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="21"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="24"/>
+      <c r="H40" s="32"/>
+      <c r="I40" s="27"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A41" s="13"/>
-      <c r="B41" s="14"/>
-      <c r="C41" s="14"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="14"/>
-      <c r="G41" s="14"/>
-      <c r="H41" s="14"/>
-      <c r="I41" s="15"/>
+      <c r="A41" s="11"/>
+      <c r="B41" s="12"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="20"/>
+      <c r="G41" s="23"/>
+      <c r="H41" s="31"/>
+      <c r="I41" s="26"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A42" s="10"/>
-      <c r="B42" s="11"/>
-      <c r="C42" s="11"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="11"/>
-      <c r="F42" s="11"/>
-      <c r="G42" s="11"/>
-      <c r="H42" s="11"/>
-      <c r="I42" s="12"/>
+      <c r="A42" s="9"/>
+      <c r="B42" s="10"/>
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21"/>
+      <c r="G42" s="24"/>
+      <c r="H42" s="32"/>
+      <c r="I42" s="27"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A43" s="13"/>
-      <c r="B43" s="14"/>
-      <c r="C43" s="14"/>
-      <c r="D43" s="14"/>
-      <c r="E43" s="14"/>
-      <c r="F43" s="14"/>
-      <c r="G43" s="14"/>
-      <c r="H43" s="14"/>
-      <c r="I43" s="15"/>
+      <c r="A43" s="11"/>
+      <c r="B43" s="12"/>
+      <c r="C43" s="20"/>
+      <c r="D43" s="20"/>
+      <c r="E43" s="20"/>
+      <c r="F43" s="20"/>
+      <c r="G43" s="23"/>
+      <c r="H43" s="31"/>
+      <c r="I43" s="26"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A44" s="10"/>
-      <c r="B44" s="11"/>
-      <c r="C44" s="11"/>
-      <c r="D44" s="11"/>
-      <c r="E44" s="11"/>
-      <c r="F44" s="11"/>
-      <c r="G44" s="11"/>
-      <c r="H44" s="11"/>
-      <c r="I44" s="12"/>
+      <c r="A44" s="9"/>
+      <c r="B44" s="10"/>
+      <c r="C44" s="21"/>
+      <c r="D44" s="21"/>
+      <c r="E44" s="21"/>
+      <c r="F44" s="21"/>
+      <c r="G44" s="24"/>
+      <c r="H44" s="32"/>
+      <c r="I44" s="27"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A45" s="13"/>
-      <c r="B45" s="14"/>
-      <c r="C45" s="14"/>
-      <c r="D45" s="14"/>
-      <c r="E45" s="14"/>
-      <c r="F45" s="14"/>
-      <c r="G45" s="14"/>
-      <c r="H45" s="14"/>
-      <c r="I45" s="15"/>
+      <c r="A45" s="11"/>
+      <c r="B45" s="12"/>
+      <c r="C45" s="20"/>
+      <c r="D45" s="20"/>
+      <c r="E45" s="20"/>
+      <c r="F45" s="20"/>
+      <c r="G45" s="23"/>
+      <c r="H45" s="31"/>
+      <c r="I45" s="26"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A46" s="10"/>
-      <c r="B46" s="11"/>
-      <c r="C46" s="11"/>
-      <c r="D46" s="11"/>
-      <c r="E46" s="11"/>
-      <c r="F46" s="11"/>
-      <c r="G46" s="11"/>
-      <c r="H46" s="11"/>
-      <c r="I46" s="12"/>
+      <c r="A46" s="9"/>
+      <c r="B46" s="10"/>
+      <c r="C46" s="21"/>
+      <c r="D46" s="21"/>
+      <c r="E46" s="21"/>
+      <c r="F46" s="21"/>
+      <c r="G46" s="24"/>
+      <c r="H46" s="32"/>
+      <c r="I46" s="27"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A47" s="13"/>
-      <c r="B47" s="14"/>
-      <c r="C47" s="14"/>
-      <c r="D47" s="14"/>
-      <c r="E47" s="14"/>
-      <c r="F47" s="14"/>
-      <c r="G47" s="14"/>
-      <c r="H47" s="14"/>
-      <c r="I47" s="15"/>
+      <c r="A47" s="11"/>
+      <c r="B47" s="12"/>
+      <c r="C47" s="20"/>
+      <c r="D47" s="20"/>
+      <c r="E47" s="20"/>
+      <c r="F47" s="20"/>
+      <c r="G47" s="23"/>
+      <c r="H47" s="31"/>
+      <c r="I47" s="26"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A48" s="10"/>
-      <c r="B48" s="11"/>
-      <c r="C48" s="11"/>
-      <c r="D48" s="11"/>
-      <c r="E48" s="11"/>
-      <c r="F48" s="11"/>
-      <c r="G48" s="11"/>
-      <c r="H48" s="11"/>
-      <c r="I48" s="12"/>
+      <c r="A48" s="9"/>
+      <c r="B48" s="10"/>
+      <c r="C48" s="21"/>
+      <c r="D48" s="21"/>
+      <c r="E48" s="21"/>
+      <c r="F48" s="21"/>
+      <c r="G48" s="24"/>
+      <c r="H48" s="32"/>
+      <c r="I48" s="27"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A49" s="13"/>
-      <c r="B49" s="14"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
-      <c r="H49" s="14"/>
-      <c r="I49" s="15"/>
+      <c r="A49" s="11"/>
+      <c r="B49" s="12"/>
+      <c r="C49" s="20"/>
+      <c r="D49" s="20"/>
+      <c r="E49" s="20"/>
+      <c r="F49" s="20"/>
+      <c r="G49" s="23"/>
+      <c r="H49" s="31"/>
+      <c r="I49" s="26"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A50" s="10"/>
-      <c r="B50" s="11"/>
-      <c r="C50" s="11"/>
-      <c r="D50" s="11"/>
-      <c r="E50" s="11"/>
-      <c r="F50" s="11"/>
-      <c r="G50" s="11"/>
-      <c r="H50" s="11"/>
-      <c r="I50" s="12"/>
+      <c r="A50" s="9"/>
+      <c r="B50" s="10"/>
+      <c r="C50" s="21"/>
+      <c r="D50" s="21"/>
+      <c r="E50" s="21"/>
+      <c r="F50" s="21"/>
+      <c r="G50" s="24"/>
+      <c r="H50" s="32"/>
+      <c r="I50" s="27"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="7"/>
       <c r="B51" s="8"/>
-      <c r="C51" s="8"/>
-      <c r="D51" s="8"/>
-      <c r="E51" s="8"/>
-      <c r="F51" s="8"/>
-      <c r="G51" s="8"/>
-      <c r="H51" s="8"/>
-      <c r="I51" s="9"/>
+      <c r="C51" s="22"/>
+      <c r="D51" s="22"/>
+      <c r="E51" s="22"/>
+      <c r="F51" s="22"/>
+      <c r="G51" s="25"/>
+      <c r="H51" s="33"/>
+      <c r="I51" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Display an message in xlsx table to don't set Totel line in the excel file of logements
</commit_message>
<xml_diff>
--- a/static/files/logements.xlsx
+++ b/static/files/logements.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasoudard/workspace/beta.gouv.fr/apilos/static/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F34024BA-0785-D74C-A261-99C525871DE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B3FCFED-12B3-4140-8933-88B3408D72CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34480" yWindow="4440" windowWidth="27020" windowHeight="16440" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Ici quelques explications</t>
   </si>
@@ -128,6 +128,12 @@
   </si>
   <si>
     <t>5. Vérifier le contenu téléversé dans l'application et enregistrer en cliquant sur le bouton 'Enregistrer et Suivant'</t>
+  </si>
+  <si>
+    <t>Attention : ne pas mettre la ligne Total dans ce tableau</t>
+  </si>
+  <si>
+    <t>elle sera calculée automatiquement lors de l'import des logements</t>
   </si>
 </sst>
 </file>
@@ -138,7 +144,7 @@
     <numFmt numFmtId="164" formatCode="#,##0.00\ [$€-40C]"/>
     <numFmt numFmtId="165" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -171,6 +177,14 @@
       <b/>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFC00000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -305,7 +319,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -354,6 +368,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -787,7 +802,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
         <v>13</v>
       </c>
@@ -810,6 +825,9 @@
       </c>
       <c r="I2" s="14" t="s">
         <v>19</v>
+      </c>
+      <c r="J2" s="34" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
@@ -822,6 +840,9 @@
       <c r="G3" s="21"/>
       <c r="H3" s="29"/>
       <c r="I3" s="24"/>
+      <c r="J3" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="9"/>

</xml_diff>

<commit_message>
Display an message in xlsx table to don't set Totel line in the excel file of logements (#107)
</commit_message>
<xml_diff>
--- a/static/files/logements.xlsx
+++ b/static/files/logements.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasoudard/workspace/beta.gouv.fr/apilos/static/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F34024BA-0785-D74C-A261-99C525871DE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B3FCFED-12B3-4140-8933-88B3408D72CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34480" yWindow="4440" windowWidth="27020" windowHeight="16440" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Ici quelques explications</t>
   </si>
@@ -128,6 +128,12 @@
   </si>
   <si>
     <t>5. Vérifier le contenu téléversé dans l'application et enregistrer en cliquant sur le bouton 'Enregistrer et Suivant'</t>
+  </si>
+  <si>
+    <t>Attention : ne pas mettre la ligne Total dans ce tableau</t>
+  </si>
+  <si>
+    <t>elle sera calculée automatiquement lors de l'import des logements</t>
   </si>
 </sst>
 </file>
@@ -138,7 +144,7 @@
     <numFmt numFmtId="164" formatCode="#,##0.00\ [$€-40C]"/>
     <numFmt numFmtId="165" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -171,6 +177,14 @@
       <b/>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFC00000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -305,7 +319,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -354,6 +368,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -787,7 +802,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
         <v>13</v>
       </c>
@@ -810,6 +825,9 @@
       </c>
       <c r="I2" s="14" t="s">
         <v>19</v>
+      </c>
+      <c r="J2" s="34" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
@@ -822,6 +840,9 @@
       <c r="G3" s="21"/>
       <c r="H3" s="29"/>
       <c r="I3" s="24"/>
+      <c r="J3" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="9"/>

</xml_diff>

<commit_message>
maxinum in maximum in xls file
</commit_message>
<xml_diff>
--- a/static/files/logements.xlsx
+++ b/static/files/logements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasoudard/workspace/beta.gouv.fr/apilos/static/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B3FCFED-12B3-4140-8933-88B3408D72CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{010CD73E-B016-E748-92F2-005EE1D5224B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34480" yWindow="4440" windowWidth="27020" windowHeight="16440" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
+    <workbookView xWindow="1000" yWindow="500" windowWidth="27800" windowHeight="17500" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Logements" sheetId="1" r:id="rId1"/>
@@ -117,23 +117,23 @@
 (article R.111-2)</t>
   </si>
   <si>
-    <t>Loyer maxinum en € par m² de surface utile</t>
-  </si>
-  <si>
-    <t>Loyer maxinum du logement en €
+    <t>2. Modifier à votre guise le fichier</t>
+  </si>
+  <si>
+    <t>5. Vérifier le contenu téléversé dans l'application et enregistrer en cliquant sur le bouton 'Enregistrer et Suivant'</t>
+  </si>
+  <si>
+    <t>Attention : ne pas mettre la ligne Total dans ce tableau</t>
+  </si>
+  <si>
+    <t>elle sera calculée automatiquement lors de l'import des logements</t>
+  </si>
+  <si>
+    <t>Loyer maximum en € par m² de surface utile</t>
+  </si>
+  <si>
+    <t>Loyer maximum du logement en €
 (col 4 * col 5 * col 6)</t>
-  </si>
-  <si>
-    <t>2. Modifier à votre guise le fichier</t>
-  </si>
-  <si>
-    <t>5. Vérifier le contenu téléversé dans l'application et enregistrer en cliquant sur le bouton 'Enregistrer et Suivant'</t>
-  </si>
-  <si>
-    <t>Attention : ne pas mettre la ligne Total dans ce tableau</t>
-  </si>
-  <si>
-    <t>elle sera calculée automatiquement lors de l'import des logements</t>
   </si>
 </sst>
 </file>
@@ -362,13 +362,13 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -765,7 +765,7 @@
   <dimension ref="A1:Q51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -793,27 +793,27 @@
         <v>21</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="H1" s="16" t="s">
         <v>6</v>
       </c>
       <c r="I1" s="17" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="33"/>
+      <c r="B2" s="34"/>
       <c r="C2" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="33" t="s">
+      <c r="D2" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="33"/>
+      <c r="E2" s="34"/>
       <c r="F2" s="13" t="s">
         <v>16</v>
       </c>
@@ -826,8 +826,8 @@
       <c r="I2" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="34" t="s">
-        <v>29</v>
+      <c r="J2" s="32" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
@@ -841,7 +841,7 @@
       <c r="H3" s="29"/>
       <c r="I3" s="24"/>
       <c r="J3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
@@ -1434,7 +1434,7 @@
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.2">
@@ -1449,7 +1449,7 @@
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
need 4 digits to coeficient
</commit_message>
<xml_diff>
--- a/static/files/logements.xlsx
+++ b/static/files/logements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasoudard/workspace/beta.gouv.fr/apilos/static/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C135054F-4AF9-8143-9EC4-056FAEEA0AC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD9CA2D2-A5E0-0348-9984-8DB2CCA78700}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="500" windowWidth="27800" windowHeight="17500" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Notice" sheetId="2" r:id="rId2"/>
     <sheet name="Data" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -142,7 +142,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.00\ [$€-40C]"/>
-    <numFmt numFmtId="165" formatCode="#,##0.000"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -272,19 +272,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </right>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color theme="4" tint="0.39997558519241921"/>
       </left>
@@ -315,11 +302,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39994506668294322"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -329,15 +329,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -345,30 +348,25 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -764,7 +762,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08021C90-1ACF-2A4C-A1B0-58A48A8F7007}">
   <dimension ref="A1:Q51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -801,17 +801,17 @@
       </c>
     </row>
     <row r="2" spans="1:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="34"/>
+      <c r="B2" s="31"/>
       <c r="C2" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="D2" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="34"/>
+      <c r="E2" s="31"/>
       <c r="F2" s="13" t="s">
         <v>16</v>
       </c>
@@ -824,7 +824,7 @@
       <c r="I2" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="32" t="s">
+      <c r="J2" s="24" t="s">
         <v>27</v>
       </c>
     </row>
@@ -836,8 +836,11 @@
       <c r="E3" s="18"/>
       <c r="F3" s="18"/>
       <c r="G3" s="21"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="24"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="28" t="str">
+        <f>IF(F3*G3*H3&gt;0,F3*G3*H3,"")</f>
+        <v/>
+      </c>
       <c r="J3" t="s">
         <v>28</v>
       </c>
@@ -850,8 +853,11 @@
       <c r="E4" s="19"/>
       <c r="F4" s="19"/>
       <c r="G4" s="22"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="25"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="29" t="str">
+        <f>IF(F4*G4*H4&gt;0,F4*G4*H4,"")</f>
+        <v/>
+      </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="11"/>
@@ -861,8 +867,11 @@
       <c r="E5" s="18"/>
       <c r="F5" s="18"/>
       <c r="G5" s="21"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="24"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="28" t="str">
+        <f t="shared" ref="I5:I51" si="0">IF(F5*G5*H5&gt;0,F5*G5*H5,"")</f>
+        <v/>
+      </c>
     </row>
     <row r="6" spans="1:17" ht="20" x14ac:dyDescent="0.2">
       <c r="A6" s="9"/>
@@ -872,8 +881,11 @@
       <c r="E6" s="19"/>
       <c r="F6" s="19"/>
       <c r="G6" s="22"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
       <c r="L6" s="5"/>
@@ -891,8 +903,11 @@
       <c r="E7" s="18"/>
       <c r="F7" s="18"/>
       <c r="G7" s="21"/>
-      <c r="H7" s="29"/>
-      <c r="I7" s="27"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
       <c r="L7" s="5"/>
@@ -910,8 +925,11 @@
       <c r="E8" s="19"/>
       <c r="F8" s="19"/>
       <c r="G8" s="22"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="25"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="11"/>
@@ -921,8 +939,11 @@
       <c r="E9" s="18"/>
       <c r="F9" s="18"/>
       <c r="G9" s="21"/>
-      <c r="H9" s="29"/>
-      <c r="I9" s="24"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="9"/>
@@ -932,8 +953,11 @@
       <c r="E10" s="19"/>
       <c r="F10" s="19"/>
       <c r="G10" s="22"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="25"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="11"/>
@@ -943,8 +967,11 @@
       <c r="E11" s="18"/>
       <c r="F11" s="18"/>
       <c r="G11" s="21"/>
-      <c r="H11" s="29"/>
-      <c r="I11" s="24"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="9"/>
@@ -954,8 +981,11 @@
       <c r="E12" s="19"/>
       <c r="F12" s="19"/>
       <c r="G12" s="22"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="25"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="11"/>
@@ -965,8 +995,11 @@
       <c r="E13" s="18"/>
       <c r="F13" s="18"/>
       <c r="G13" s="21"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="24"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="9"/>
@@ -976,8 +1009,11 @@
       <c r="E14" s="19"/>
       <c r="F14" s="19"/>
       <c r="G14" s="22"/>
-      <c r="H14" s="30"/>
-      <c r="I14" s="25"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="11"/>
@@ -987,8 +1023,11 @@
       <c r="E15" s="18"/>
       <c r="F15" s="18"/>
       <c r="G15" s="21"/>
-      <c r="H15" s="29"/>
-      <c r="I15" s="24"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="9"/>
@@ -998,8 +1037,11 @@
       <c r="E16" s="19"/>
       <c r="F16" s="19"/>
       <c r="G16" s="22"/>
-      <c r="H16" s="30"/>
-      <c r="I16" s="25"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="11"/>
@@ -1009,8 +1051,11 @@
       <c r="E17" s="18"/>
       <c r="F17" s="18"/>
       <c r="G17" s="21"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="24"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="9"/>
@@ -1020,8 +1065,11 @@
       <c r="E18" s="19"/>
       <c r="F18" s="19"/>
       <c r="G18" s="22"/>
-      <c r="H18" s="30"/>
-      <c r="I18" s="25"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="11"/>
@@ -1031,8 +1079,11 @@
       <c r="E19" s="18"/>
       <c r="F19" s="18"/>
       <c r="G19" s="21"/>
-      <c r="H19" s="29"/>
-      <c r="I19" s="24"/>
+      <c r="H19" s="25"/>
+      <c r="I19" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="9"/>
@@ -1042,8 +1093,11 @@
       <c r="E20" s="19"/>
       <c r="F20" s="19"/>
       <c r="G20" s="22"/>
-      <c r="H20" s="30"/>
-      <c r="I20" s="25"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="11"/>
@@ -1053,8 +1107,11 @@
       <c r="E21" s="18"/>
       <c r="F21" s="18"/>
       <c r="G21" s="21"/>
-      <c r="H21" s="29"/>
-      <c r="I21" s="24"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="9"/>
@@ -1064,8 +1121,11 @@
       <c r="E22" s="19"/>
       <c r="F22" s="19"/>
       <c r="G22" s="22"/>
-      <c r="H22" s="30"/>
-      <c r="I22" s="25"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="11"/>
@@ -1075,8 +1135,11 @@
       <c r="E23" s="18"/>
       <c r="F23" s="18"/>
       <c r="G23" s="21"/>
-      <c r="H23" s="29"/>
-      <c r="I23" s="24"/>
+      <c r="H23" s="25"/>
+      <c r="I23" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="9"/>
@@ -1086,8 +1149,11 @@
       <c r="E24" s="19"/>
       <c r="F24" s="19"/>
       <c r="G24" s="22"/>
-      <c r="H24" s="30"/>
-      <c r="I24" s="25"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="11"/>
@@ -1097,8 +1163,11 @@
       <c r="E25" s="18"/>
       <c r="F25" s="18"/>
       <c r="G25" s="21"/>
-      <c r="H25" s="29"/>
-      <c r="I25" s="24"/>
+      <c r="H25" s="25"/>
+      <c r="I25" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="9"/>
@@ -1108,8 +1177,11 @@
       <c r="E26" s="19"/>
       <c r="F26" s="19"/>
       <c r="G26" s="22"/>
-      <c r="H26" s="30"/>
-      <c r="I26" s="25"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="11"/>
@@ -1119,8 +1191,11 @@
       <c r="E27" s="18"/>
       <c r="F27" s="18"/>
       <c r="G27" s="21"/>
-      <c r="H27" s="29"/>
-      <c r="I27" s="24"/>
+      <c r="H27" s="25"/>
+      <c r="I27" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="9"/>
@@ -1130,8 +1205,11 @@
       <c r="E28" s="19"/>
       <c r="F28" s="19"/>
       <c r="G28" s="22"/>
-      <c r="H28" s="30"/>
-      <c r="I28" s="25"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="11"/>
@@ -1141,8 +1219,11 @@
       <c r="E29" s="18"/>
       <c r="F29" s="18"/>
       <c r="G29" s="21"/>
-      <c r="H29" s="29"/>
-      <c r="I29" s="24"/>
+      <c r="H29" s="25"/>
+      <c r="I29" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="9"/>
@@ -1152,8 +1233,11 @@
       <c r="E30" s="19"/>
       <c r="F30" s="19"/>
       <c r="G30" s="22"/>
-      <c r="H30" s="30"/>
-      <c r="I30" s="25"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="11"/>
@@ -1163,8 +1247,11 @@
       <c r="E31" s="18"/>
       <c r="F31" s="18"/>
       <c r="G31" s="21"/>
-      <c r="H31" s="29"/>
-      <c r="I31" s="24"/>
+      <c r="H31" s="25"/>
+      <c r="I31" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="9"/>
@@ -1174,8 +1261,11 @@
       <c r="E32" s="19"/>
       <c r="F32" s="19"/>
       <c r="G32" s="22"/>
-      <c r="H32" s="30"/>
-      <c r="I32" s="25"/>
+      <c r="H32" s="26"/>
+      <c r="I32" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="11"/>
@@ -1185,8 +1275,11 @@
       <c r="E33" s="18"/>
       <c r="F33" s="18"/>
       <c r="G33" s="21"/>
-      <c r="H33" s="29"/>
-      <c r="I33" s="24"/>
+      <c r="H33" s="25"/>
+      <c r="I33" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="9"/>
@@ -1196,8 +1289,11 @@
       <c r="E34" s="19"/>
       <c r="F34" s="19"/>
       <c r="G34" s="22"/>
-      <c r="H34" s="30"/>
-      <c r="I34" s="25"/>
+      <c r="H34" s="26"/>
+      <c r="I34" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="11"/>
@@ -1207,8 +1303,11 @@
       <c r="E35" s="18"/>
       <c r="F35" s="18"/>
       <c r="G35" s="21"/>
-      <c r="H35" s="29"/>
-      <c r="I35" s="24"/>
+      <c r="H35" s="25"/>
+      <c r="I35" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="9"/>
@@ -1218,8 +1317,11 @@
       <c r="E36" s="19"/>
       <c r="F36" s="19"/>
       <c r="G36" s="22"/>
-      <c r="H36" s="30"/>
-      <c r="I36" s="25"/>
+      <c r="H36" s="26"/>
+      <c r="I36" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="11"/>
@@ -1229,8 +1331,11 @@
       <c r="E37" s="18"/>
       <c r="F37" s="18"/>
       <c r="G37" s="21"/>
-      <c r="H37" s="29"/>
-      <c r="I37" s="24"/>
+      <c r="H37" s="25"/>
+      <c r="I37" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="9"/>
@@ -1240,8 +1345,11 @@
       <c r="E38" s="19"/>
       <c r="F38" s="19"/>
       <c r="G38" s="22"/>
-      <c r="H38" s="30"/>
-      <c r="I38" s="25"/>
+      <c r="H38" s="26"/>
+      <c r="I38" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="11"/>
@@ -1251,8 +1359,11 @@
       <c r="E39" s="18"/>
       <c r="F39" s="18"/>
       <c r="G39" s="21"/>
-      <c r="H39" s="29"/>
-      <c r="I39" s="24"/>
+      <c r="H39" s="25"/>
+      <c r="I39" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="9"/>
@@ -1262,8 +1373,11 @@
       <c r="E40" s="19"/>
       <c r="F40" s="19"/>
       <c r="G40" s="22"/>
-      <c r="H40" s="30"/>
-      <c r="I40" s="25"/>
+      <c r="H40" s="26"/>
+      <c r="I40" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="11"/>
@@ -1273,8 +1387,11 @@
       <c r="E41" s="18"/>
       <c r="F41" s="18"/>
       <c r="G41" s="21"/>
-      <c r="H41" s="29"/>
-      <c r="I41" s="24"/>
+      <c r="H41" s="25"/>
+      <c r="I41" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="9"/>
@@ -1284,8 +1401,11 @@
       <c r="E42" s="19"/>
       <c r="F42" s="19"/>
       <c r="G42" s="22"/>
-      <c r="H42" s="30"/>
-      <c r="I42" s="25"/>
+      <c r="H42" s="26"/>
+      <c r="I42" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="11"/>
@@ -1295,8 +1415,11 @@
       <c r="E43" s="18"/>
       <c r="F43" s="18"/>
       <c r="G43" s="21"/>
-      <c r="H43" s="29"/>
-      <c r="I43" s="24"/>
+      <c r="H43" s="25"/>
+      <c r="I43" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="9"/>
@@ -1306,8 +1429,11 @@
       <c r="E44" s="19"/>
       <c r="F44" s="19"/>
       <c r="G44" s="22"/>
-      <c r="H44" s="30"/>
-      <c r="I44" s="25"/>
+      <c r="H44" s="26"/>
+      <c r="I44" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="11"/>
@@ -1317,8 +1443,11 @@
       <c r="E45" s="18"/>
       <c r="F45" s="18"/>
       <c r="G45" s="21"/>
-      <c r="H45" s="29"/>
-      <c r="I45" s="24"/>
+      <c r="H45" s="25"/>
+      <c r="I45" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="9"/>
@@ -1328,8 +1457,11 @@
       <c r="E46" s="19"/>
       <c r="F46" s="19"/>
       <c r="G46" s="22"/>
-      <c r="H46" s="30"/>
-      <c r="I46" s="25"/>
+      <c r="H46" s="26"/>
+      <c r="I46" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="11"/>
@@ -1339,8 +1471,11 @@
       <c r="E47" s="18"/>
       <c r="F47" s="18"/>
       <c r="G47" s="21"/>
-      <c r="H47" s="29"/>
-      <c r="I47" s="24"/>
+      <c r="H47" s="25"/>
+      <c r="I47" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="9"/>
@@ -1350,8 +1485,11 @@
       <c r="E48" s="19"/>
       <c r="F48" s="19"/>
       <c r="G48" s="22"/>
-      <c r="H48" s="30"/>
-      <c r="I48" s="25"/>
+      <c r="H48" s="26"/>
+      <c r="I48" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="11"/>
@@ -1361,8 +1499,11 @@
       <c r="E49" s="18"/>
       <c r="F49" s="18"/>
       <c r="G49" s="21"/>
-      <c r="H49" s="29"/>
-      <c r="I49" s="24"/>
+      <c r="H49" s="25"/>
+      <c r="I49" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="9"/>
@@ -1372,8 +1513,11 @@
       <c r="E50" s="19"/>
       <c r="F50" s="19"/>
       <c r="G50" s="22"/>
-      <c r="H50" s="30"/>
-      <c r="I50" s="25"/>
+      <c r="H50" s="26"/>
+      <c r="I50" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="7"/>
@@ -1383,8 +1527,11 @@
       <c r="E51" s="20"/>
       <c r="F51" s="20"/>
       <c r="G51" s="23"/>
-      <c r="H51" s="31"/>
-      <c r="I51" s="28"/>
+      <c r="H51" s="27"/>
+      <c r="I51" s="32" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
need 4 digits to coeficient (#132)
</commit_message>
<xml_diff>
--- a/static/files/logements.xlsx
+++ b/static/files/logements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasoudard/workspace/beta.gouv.fr/apilos/static/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C135054F-4AF9-8143-9EC4-056FAEEA0AC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD9CA2D2-A5E0-0348-9984-8DB2CCA78700}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="500" windowWidth="27800" windowHeight="17500" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Notice" sheetId="2" r:id="rId2"/>
     <sheet name="Data" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -142,7 +142,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.00\ [$€-40C]"/>
-    <numFmt numFmtId="165" formatCode="#,##0.000"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -272,19 +272,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </right>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color theme="4" tint="0.39997558519241921"/>
       </left>
@@ -315,11 +302,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39994506668294322"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -329,15 +329,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -345,30 +348,25 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -764,7 +762,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08021C90-1ACF-2A4C-A1B0-58A48A8F7007}">
   <dimension ref="A1:Q51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -801,17 +801,17 @@
       </c>
     </row>
     <row r="2" spans="1:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="34"/>
+      <c r="B2" s="31"/>
       <c r="C2" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="D2" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="34"/>
+      <c r="E2" s="31"/>
       <c r="F2" s="13" t="s">
         <v>16</v>
       </c>
@@ -824,7 +824,7 @@
       <c r="I2" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="32" t="s">
+      <c r="J2" s="24" t="s">
         <v>27</v>
       </c>
     </row>
@@ -836,8 +836,11 @@
       <c r="E3" s="18"/>
       <c r="F3" s="18"/>
       <c r="G3" s="21"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="24"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="28" t="str">
+        <f>IF(F3*G3*H3&gt;0,F3*G3*H3,"")</f>
+        <v/>
+      </c>
       <c r="J3" t="s">
         <v>28</v>
       </c>
@@ -850,8 +853,11 @@
       <c r="E4" s="19"/>
       <c r="F4" s="19"/>
       <c r="G4" s="22"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="25"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="29" t="str">
+        <f>IF(F4*G4*H4&gt;0,F4*G4*H4,"")</f>
+        <v/>
+      </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="11"/>
@@ -861,8 +867,11 @@
       <c r="E5" s="18"/>
       <c r="F5" s="18"/>
       <c r="G5" s="21"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="24"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="28" t="str">
+        <f t="shared" ref="I5:I51" si="0">IF(F5*G5*H5&gt;0,F5*G5*H5,"")</f>
+        <v/>
+      </c>
     </row>
     <row r="6" spans="1:17" ht="20" x14ac:dyDescent="0.2">
       <c r="A6" s="9"/>
@@ -872,8 +881,11 @@
       <c r="E6" s="19"/>
       <c r="F6" s="19"/>
       <c r="G6" s="22"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
       <c r="L6" s="5"/>
@@ -891,8 +903,11 @@
       <c r="E7" s="18"/>
       <c r="F7" s="18"/>
       <c r="G7" s="21"/>
-      <c r="H7" s="29"/>
-      <c r="I7" s="27"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
       <c r="L7" s="5"/>
@@ -910,8 +925,11 @@
       <c r="E8" s="19"/>
       <c r="F8" s="19"/>
       <c r="G8" s="22"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="25"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="11"/>
@@ -921,8 +939,11 @@
       <c r="E9" s="18"/>
       <c r="F9" s="18"/>
       <c r="G9" s="21"/>
-      <c r="H9" s="29"/>
-      <c r="I9" s="24"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="9"/>
@@ -932,8 +953,11 @@
       <c r="E10" s="19"/>
       <c r="F10" s="19"/>
       <c r="G10" s="22"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="25"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="11"/>
@@ -943,8 +967,11 @@
       <c r="E11" s="18"/>
       <c r="F11" s="18"/>
       <c r="G11" s="21"/>
-      <c r="H11" s="29"/>
-      <c r="I11" s="24"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="9"/>
@@ -954,8 +981,11 @@
       <c r="E12" s="19"/>
       <c r="F12" s="19"/>
       <c r="G12" s="22"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="25"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="11"/>
@@ -965,8 +995,11 @@
       <c r="E13" s="18"/>
       <c r="F13" s="18"/>
       <c r="G13" s="21"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="24"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="9"/>
@@ -976,8 +1009,11 @@
       <c r="E14" s="19"/>
       <c r="F14" s="19"/>
       <c r="G14" s="22"/>
-      <c r="H14" s="30"/>
-      <c r="I14" s="25"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="11"/>
@@ -987,8 +1023,11 @@
       <c r="E15" s="18"/>
       <c r="F15" s="18"/>
       <c r="G15" s="21"/>
-      <c r="H15" s="29"/>
-      <c r="I15" s="24"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="9"/>
@@ -998,8 +1037,11 @@
       <c r="E16" s="19"/>
       <c r="F16" s="19"/>
       <c r="G16" s="22"/>
-      <c r="H16" s="30"/>
-      <c r="I16" s="25"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="11"/>
@@ -1009,8 +1051,11 @@
       <c r="E17" s="18"/>
       <c r="F17" s="18"/>
       <c r="G17" s="21"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="24"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="9"/>
@@ -1020,8 +1065,11 @@
       <c r="E18" s="19"/>
       <c r="F18" s="19"/>
       <c r="G18" s="22"/>
-      <c r="H18" s="30"/>
-      <c r="I18" s="25"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="11"/>
@@ -1031,8 +1079,11 @@
       <c r="E19" s="18"/>
       <c r="F19" s="18"/>
       <c r="G19" s="21"/>
-      <c r="H19" s="29"/>
-      <c r="I19" s="24"/>
+      <c r="H19" s="25"/>
+      <c r="I19" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="9"/>
@@ -1042,8 +1093,11 @@
       <c r="E20" s="19"/>
       <c r="F20" s="19"/>
       <c r="G20" s="22"/>
-      <c r="H20" s="30"/>
-      <c r="I20" s="25"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="11"/>
@@ -1053,8 +1107,11 @@
       <c r="E21" s="18"/>
       <c r="F21" s="18"/>
       <c r="G21" s="21"/>
-      <c r="H21" s="29"/>
-      <c r="I21" s="24"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="9"/>
@@ -1064,8 +1121,11 @@
       <c r="E22" s="19"/>
       <c r="F22" s="19"/>
       <c r="G22" s="22"/>
-      <c r="H22" s="30"/>
-      <c r="I22" s="25"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="11"/>
@@ -1075,8 +1135,11 @@
       <c r="E23" s="18"/>
       <c r="F23" s="18"/>
       <c r="G23" s="21"/>
-      <c r="H23" s="29"/>
-      <c r="I23" s="24"/>
+      <c r="H23" s="25"/>
+      <c r="I23" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="9"/>
@@ -1086,8 +1149,11 @@
       <c r="E24" s="19"/>
       <c r="F24" s="19"/>
       <c r="G24" s="22"/>
-      <c r="H24" s="30"/>
-      <c r="I24" s="25"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="11"/>
@@ -1097,8 +1163,11 @@
       <c r="E25" s="18"/>
       <c r="F25" s="18"/>
       <c r="G25" s="21"/>
-      <c r="H25" s="29"/>
-      <c r="I25" s="24"/>
+      <c r="H25" s="25"/>
+      <c r="I25" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="9"/>
@@ -1108,8 +1177,11 @@
       <c r="E26" s="19"/>
       <c r="F26" s="19"/>
       <c r="G26" s="22"/>
-      <c r="H26" s="30"/>
-      <c r="I26" s="25"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="11"/>
@@ -1119,8 +1191,11 @@
       <c r="E27" s="18"/>
       <c r="F27" s="18"/>
       <c r="G27" s="21"/>
-      <c r="H27" s="29"/>
-      <c r="I27" s="24"/>
+      <c r="H27" s="25"/>
+      <c r="I27" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="9"/>
@@ -1130,8 +1205,11 @@
       <c r="E28" s="19"/>
       <c r="F28" s="19"/>
       <c r="G28" s="22"/>
-      <c r="H28" s="30"/>
-      <c r="I28" s="25"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="11"/>
@@ -1141,8 +1219,11 @@
       <c r="E29" s="18"/>
       <c r="F29" s="18"/>
       <c r="G29" s="21"/>
-      <c r="H29" s="29"/>
-      <c r="I29" s="24"/>
+      <c r="H29" s="25"/>
+      <c r="I29" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="9"/>
@@ -1152,8 +1233,11 @@
       <c r="E30" s="19"/>
       <c r="F30" s="19"/>
       <c r="G30" s="22"/>
-      <c r="H30" s="30"/>
-      <c r="I30" s="25"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="11"/>
@@ -1163,8 +1247,11 @@
       <c r="E31" s="18"/>
       <c r="F31" s="18"/>
       <c r="G31" s="21"/>
-      <c r="H31" s="29"/>
-      <c r="I31" s="24"/>
+      <c r="H31" s="25"/>
+      <c r="I31" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="9"/>
@@ -1174,8 +1261,11 @@
       <c r="E32" s="19"/>
       <c r="F32" s="19"/>
       <c r="G32" s="22"/>
-      <c r="H32" s="30"/>
-      <c r="I32" s="25"/>
+      <c r="H32" s="26"/>
+      <c r="I32" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="11"/>
@@ -1185,8 +1275,11 @@
       <c r="E33" s="18"/>
       <c r="F33" s="18"/>
       <c r="G33" s="21"/>
-      <c r="H33" s="29"/>
-      <c r="I33" s="24"/>
+      <c r="H33" s="25"/>
+      <c r="I33" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="9"/>
@@ -1196,8 +1289,11 @@
       <c r="E34" s="19"/>
       <c r="F34" s="19"/>
       <c r="G34" s="22"/>
-      <c r="H34" s="30"/>
-      <c r="I34" s="25"/>
+      <c r="H34" s="26"/>
+      <c r="I34" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="11"/>
@@ -1207,8 +1303,11 @@
       <c r="E35" s="18"/>
       <c r="F35" s="18"/>
       <c r="G35" s="21"/>
-      <c r="H35" s="29"/>
-      <c r="I35" s="24"/>
+      <c r="H35" s="25"/>
+      <c r="I35" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="9"/>
@@ -1218,8 +1317,11 @@
       <c r="E36" s="19"/>
       <c r="F36" s="19"/>
       <c r="G36" s="22"/>
-      <c r="H36" s="30"/>
-      <c r="I36" s="25"/>
+      <c r="H36" s="26"/>
+      <c r="I36" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="11"/>
@@ -1229,8 +1331,11 @@
       <c r="E37" s="18"/>
       <c r="F37" s="18"/>
       <c r="G37" s="21"/>
-      <c r="H37" s="29"/>
-      <c r="I37" s="24"/>
+      <c r="H37" s="25"/>
+      <c r="I37" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="9"/>
@@ -1240,8 +1345,11 @@
       <c r="E38" s="19"/>
       <c r="F38" s="19"/>
       <c r="G38" s="22"/>
-      <c r="H38" s="30"/>
-      <c r="I38" s="25"/>
+      <c r="H38" s="26"/>
+      <c r="I38" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="11"/>
@@ -1251,8 +1359,11 @@
       <c r="E39" s="18"/>
       <c r="F39" s="18"/>
       <c r="G39" s="21"/>
-      <c r="H39" s="29"/>
-      <c r="I39" s="24"/>
+      <c r="H39" s="25"/>
+      <c r="I39" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="9"/>
@@ -1262,8 +1373,11 @@
       <c r="E40" s="19"/>
       <c r="F40" s="19"/>
       <c r="G40" s="22"/>
-      <c r="H40" s="30"/>
-      <c r="I40" s="25"/>
+      <c r="H40" s="26"/>
+      <c r="I40" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="11"/>
@@ -1273,8 +1387,11 @@
       <c r="E41" s="18"/>
       <c r="F41" s="18"/>
       <c r="G41" s="21"/>
-      <c r="H41" s="29"/>
-      <c r="I41" s="24"/>
+      <c r="H41" s="25"/>
+      <c r="I41" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="9"/>
@@ -1284,8 +1401,11 @@
       <c r="E42" s="19"/>
       <c r="F42" s="19"/>
       <c r="G42" s="22"/>
-      <c r="H42" s="30"/>
-      <c r="I42" s="25"/>
+      <c r="H42" s="26"/>
+      <c r="I42" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="11"/>
@@ -1295,8 +1415,11 @@
       <c r="E43" s="18"/>
       <c r="F43" s="18"/>
       <c r="G43" s="21"/>
-      <c r="H43" s="29"/>
-      <c r="I43" s="24"/>
+      <c r="H43" s="25"/>
+      <c r="I43" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="9"/>
@@ -1306,8 +1429,11 @@
       <c r="E44" s="19"/>
       <c r="F44" s="19"/>
       <c r="G44" s="22"/>
-      <c r="H44" s="30"/>
-      <c r="I44" s="25"/>
+      <c r="H44" s="26"/>
+      <c r="I44" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="11"/>
@@ -1317,8 +1443,11 @@
       <c r="E45" s="18"/>
       <c r="F45" s="18"/>
       <c r="G45" s="21"/>
-      <c r="H45" s="29"/>
-      <c r="I45" s="24"/>
+      <c r="H45" s="25"/>
+      <c r="I45" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="9"/>
@@ -1328,8 +1457,11 @@
       <c r="E46" s="19"/>
       <c r="F46" s="19"/>
       <c r="G46" s="22"/>
-      <c r="H46" s="30"/>
-      <c r="I46" s="25"/>
+      <c r="H46" s="26"/>
+      <c r="I46" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="11"/>
@@ -1339,8 +1471,11 @@
       <c r="E47" s="18"/>
       <c r="F47" s="18"/>
       <c r="G47" s="21"/>
-      <c r="H47" s="29"/>
-      <c r="I47" s="24"/>
+      <c r="H47" s="25"/>
+      <c r="I47" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="9"/>
@@ -1350,8 +1485,11 @@
       <c r="E48" s="19"/>
       <c r="F48" s="19"/>
       <c r="G48" s="22"/>
-      <c r="H48" s="30"/>
-      <c r="I48" s="25"/>
+      <c r="H48" s="26"/>
+      <c r="I48" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="11"/>
@@ -1361,8 +1499,11 @@
       <c r="E49" s="18"/>
       <c r="F49" s="18"/>
       <c r="G49" s="21"/>
-      <c r="H49" s="29"/>
-      <c r="I49" s="24"/>
+      <c r="H49" s="25"/>
+      <c r="I49" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="9"/>
@@ -1372,8 +1513,11 @@
       <c r="E50" s="19"/>
       <c r="F50" s="19"/>
       <c r="G50" s="22"/>
-      <c r="H50" s="30"/>
-      <c r="I50" s="25"/>
+      <c r="H50" s="26"/>
+      <c r="I50" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="7"/>
@@ -1383,8 +1527,11 @@
       <c r="E51" s="20"/>
       <c r="F51" s="20"/>
       <c r="G51" s="23"/>
-      <c r="H51" s="31"/>
-      <c r="I51" s="28"/>
+      <c r="H51" s="27"/>
+      <c r="I51" s="32" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
s524: update article number of surface habitable
</commit_message>
<xml_diff>
--- a/static/files/logements.xlsx
+++ b/static/files/logements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marjo\Desktop\HD\Beta-Gouv\apilos\static\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasoudard/workspace/beta.gouv.fr/apilos/static/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8951AF2-4287-4B42-8022-248C7DD1E1AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1FA46CE-2510-D94A-BDD3-0EFF9DF2D415}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
+    <workbookView xWindow="1240" yWindow="500" windowWidth="27560" windowHeight="16440" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Logements" sheetId="1" r:id="rId1"/>
@@ -113,10 +113,6 @@
 Réelle</t>
   </si>
   <si>
-    <t>Surface habitable
-(article R.111-2)</t>
-  </si>
-  <si>
     <t>2. Modifier à votre guise le fichier</t>
   </si>
   <si>
@@ -143,6 +139,10 @@
   </si>
   <si>
     <t>lignes data</t>
+  </si>
+  <si>
+    <t>Surface habitable
+(article R.156-1)</t>
   </si>
 </sst>
 </file>
@@ -532,7 +532,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -831,16 +831,16 @@
   <dimension ref="A1:Q52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.75" customWidth="1"/>
-    <col min="2" max="9" width="20.875" customWidth="1"/>
+    <col min="1" max="1" width="29.6640625" customWidth="1"/>
+    <col min="2" max="9" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>20</v>
       </c>
@@ -848,7 +848,7 @@
         <v>5</v>
       </c>
       <c r="C1" s="36" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="D1" s="36" t="s">
         <v>23</v>
@@ -860,18 +860,18 @@
         <v>21</v>
       </c>
       <c r="G1" s="36" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H1" s="16" t="s">
         <v>6</v>
       </c>
       <c r="I1" s="38" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="102" x14ac:dyDescent="0.2">
+      <c r="A2" s="30" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
-        <v>31</v>
       </c>
       <c r="B2" s="37"/>
       <c r="C2" s="37"/>
@@ -880,11 +880,11 @@
       <c r="F2" s="37"/>
       <c r="G2" s="37"/>
       <c r="H2" s="31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I2" s="39"/>
     </row>
-    <row r="3" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="s">
         <v>13</v>
       </c>
@@ -909,10 +909,10 @@
         <v>19</v>
       </c>
       <c r="J3" s="23" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="11"/>
       <c r="B4" s="12"/>
       <c r="C4" s="17"/>
@@ -926,10 +926,10 @@
         <v/>
       </c>
       <c r="J4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="9"/>
       <c r="B5" s="10"/>
       <c r="C5" s="18"/>
@@ -943,7 +943,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="11"/>
       <c r="B6" s="12"/>
       <c r="C6" s="17"/>
@@ -957,7 +957,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" ht="20" x14ac:dyDescent="0.2">
       <c r="A7" s="9"/>
       <c r="B7" s="10"/>
       <c r="C7" s="18"/>
@@ -979,7 +979,7 @@
       <c r="P7" s="6"/>
       <c r="Q7" s="6"/>
     </row>
-    <row r="8" spans="1:17" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" ht="20" x14ac:dyDescent="0.2">
       <c r="A8" s="11"/>
       <c r="B8" s="12"/>
       <c r="C8" s="17"/>
@@ -1001,7 +1001,7 @@
       <c r="P8" s="6"/>
       <c r="Q8" s="6"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="9"/>
       <c r="B9" s="10"/>
       <c r="C9" s="18"/>
@@ -1015,7 +1015,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="11"/>
       <c r="B10" s="12"/>
       <c r="C10" s="17"/>
@@ -1029,7 +1029,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="9"/>
       <c r="B11" s="10"/>
       <c r="C11" s="18"/>
@@ -1043,7 +1043,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="11"/>
       <c r="B12" s="12"/>
       <c r="C12" s="17"/>
@@ -1057,7 +1057,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="9"/>
       <c r="B13" s="10"/>
       <c r="C13" s="18"/>
@@ -1071,7 +1071,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="11"/>
       <c r="B14" s="12"/>
       <c r="C14" s="17"/>
@@ -1085,7 +1085,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="9"/>
       <c r="B15" s="10"/>
       <c r="C15" s="18"/>
@@ -1099,7 +1099,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="11"/>
       <c r="B16" s="12"/>
       <c r="C16" s="17"/>
@@ -1113,7 +1113,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="9"/>
       <c r="B17" s="10"/>
       <c r="C17" s="18"/>
@@ -1127,7 +1127,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="11"/>
       <c r="B18" s="12"/>
       <c r="C18" s="17"/>
@@ -1141,7 +1141,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="9"/>
       <c r="B19" s="10"/>
       <c r="C19" s="18"/>
@@ -1155,7 +1155,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="11"/>
       <c r="B20" s="12"/>
       <c r="C20" s="17"/>
@@ -1169,7 +1169,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="9"/>
       <c r="B21" s="10"/>
       <c r="C21" s="18"/>
@@ -1183,7 +1183,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="11"/>
       <c r="B22" s="12"/>
       <c r="C22" s="17"/>
@@ -1197,7 +1197,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="9"/>
       <c r="B23" s="10"/>
       <c r="C23" s="18"/>
@@ -1211,7 +1211,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="11"/>
       <c r="B24" s="12"/>
       <c r="C24" s="17"/>
@@ -1225,7 +1225,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="9"/>
       <c r="B25" s="10"/>
       <c r="C25" s="18"/>
@@ -1239,7 +1239,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="11"/>
       <c r="B26" s="12"/>
       <c r="C26" s="17"/>
@@ -1253,7 +1253,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="9"/>
       <c r="B27" s="10"/>
       <c r="C27" s="18"/>
@@ -1267,7 +1267,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="11"/>
       <c r="B28" s="12"/>
       <c r="C28" s="17"/>
@@ -1281,7 +1281,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="9"/>
       <c r="B29" s="10"/>
       <c r="C29" s="18"/>
@@ -1295,7 +1295,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="11"/>
       <c r="B30" s="12"/>
       <c r="C30" s="17"/>
@@ -1309,7 +1309,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="9"/>
       <c r="B31" s="10"/>
       <c r="C31" s="18"/>
@@ -1323,7 +1323,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="11"/>
       <c r="B32" s="12"/>
       <c r="C32" s="17"/>
@@ -1337,7 +1337,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="9"/>
       <c r="B33" s="10"/>
       <c r="C33" s="18"/>
@@ -1351,7 +1351,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="11"/>
       <c r="B34" s="12"/>
       <c r="C34" s="17"/>
@@ -1365,7 +1365,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="9"/>
       <c r="B35" s="10"/>
       <c r="C35" s="18"/>
@@ -1379,7 +1379,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="11"/>
       <c r="B36" s="12"/>
       <c r="C36" s="17"/>
@@ -1393,7 +1393,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="9"/>
       <c r="B37" s="10"/>
       <c r="C37" s="18"/>
@@ -1407,7 +1407,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="11"/>
       <c r="B38" s="12"/>
       <c r="C38" s="17"/>
@@ -1421,7 +1421,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="9"/>
       <c r="B39" s="10"/>
       <c r="C39" s="18"/>
@@ -1435,7 +1435,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="11"/>
       <c r="B40" s="12"/>
       <c r="C40" s="17"/>
@@ -1449,7 +1449,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="9"/>
       <c r="B41" s="10"/>
       <c r="C41" s="18"/>
@@ -1463,7 +1463,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="11"/>
       <c r="B42" s="12"/>
       <c r="C42" s="17"/>
@@ -1477,7 +1477,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="9"/>
       <c r="B43" s="10"/>
       <c r="C43" s="18"/>
@@ -1491,7 +1491,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="11"/>
       <c r="B44" s="12"/>
       <c r="C44" s="17"/>
@@ -1505,7 +1505,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="9"/>
       <c r="B45" s="10"/>
       <c r="C45" s="18"/>
@@ -1519,7 +1519,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="11"/>
       <c r="B46" s="12"/>
       <c r="C46" s="17"/>
@@ -1533,7 +1533,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="9"/>
       <c r="B47" s="10"/>
       <c r="C47" s="18"/>
@@ -1547,7 +1547,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="11"/>
       <c r="B48" s="12"/>
       <c r="C48" s="17"/>
@@ -1561,7 +1561,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="9"/>
       <c r="B49" s="10"/>
       <c r="C49" s="18"/>
@@ -1575,7 +1575,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="11"/>
       <c r="B50" s="12"/>
       <c r="C50" s="17"/>
@@ -1589,7 +1589,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="9"/>
       <c r="B51" s="10"/>
       <c r="C51" s="18"/>
@@ -1603,7 +1603,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="7"/>
       <c r="B52" s="8"/>
       <c r="C52" s="19"/>
@@ -1653,43 +1653,43 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.5" customWidth="1"/>
     <col min="2" max="2" width="67" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>4</v>
       </c>
@@ -1708,20 +1708,20 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="42.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E1" s="32" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -1729,27 +1729,27 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
s524: update article number of surface habitable (#276)
</commit_message>
<xml_diff>
--- a/static/files/logements.xlsx
+++ b/static/files/logements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marjo\Desktop\HD\Beta-Gouv\apilos\static\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasoudard/workspace/beta.gouv.fr/apilos/static/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8951AF2-4287-4B42-8022-248C7DD1E1AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1FA46CE-2510-D94A-BDD3-0EFF9DF2D415}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
+    <workbookView xWindow="1240" yWindow="500" windowWidth="27560" windowHeight="16440" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Logements" sheetId="1" r:id="rId1"/>
@@ -113,10 +113,6 @@
 Réelle</t>
   </si>
   <si>
-    <t>Surface habitable
-(article R.111-2)</t>
-  </si>
-  <si>
     <t>2. Modifier à votre guise le fichier</t>
   </si>
   <si>
@@ -143,6 +139,10 @@
   </si>
   <si>
     <t>lignes data</t>
+  </si>
+  <si>
+    <t>Surface habitable
+(article R.156-1)</t>
   </si>
 </sst>
 </file>
@@ -532,7 +532,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -831,16 +831,16 @@
   <dimension ref="A1:Q52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.75" customWidth="1"/>
-    <col min="2" max="9" width="20.875" customWidth="1"/>
+    <col min="1" max="1" width="29.6640625" customWidth="1"/>
+    <col min="2" max="9" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>20</v>
       </c>
@@ -848,7 +848,7 @@
         <v>5</v>
       </c>
       <c r="C1" s="36" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="D1" s="36" t="s">
         <v>23</v>
@@ -860,18 +860,18 @@
         <v>21</v>
       </c>
       <c r="G1" s="36" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H1" s="16" t="s">
         <v>6</v>
       </c>
       <c r="I1" s="38" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="102" x14ac:dyDescent="0.2">
+      <c r="A2" s="30" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
-        <v>31</v>
       </c>
       <c r="B2" s="37"/>
       <c r="C2" s="37"/>
@@ -880,11 +880,11 @@
       <c r="F2" s="37"/>
       <c r="G2" s="37"/>
       <c r="H2" s="31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I2" s="39"/>
     </row>
-    <row r="3" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="s">
         <v>13</v>
       </c>
@@ -909,10 +909,10 @@
         <v>19</v>
       </c>
       <c r="J3" s="23" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="11"/>
       <c r="B4" s="12"/>
       <c r="C4" s="17"/>
@@ -926,10 +926,10 @@
         <v/>
       </c>
       <c r="J4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="9"/>
       <c r="B5" s="10"/>
       <c r="C5" s="18"/>
@@ -943,7 +943,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="11"/>
       <c r="B6" s="12"/>
       <c r="C6" s="17"/>
@@ -957,7 +957,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" ht="20" x14ac:dyDescent="0.2">
       <c r="A7" s="9"/>
       <c r="B7" s="10"/>
       <c r="C7" s="18"/>
@@ -979,7 +979,7 @@
       <c r="P7" s="6"/>
       <c r="Q7" s="6"/>
     </row>
-    <row r="8" spans="1:17" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" ht="20" x14ac:dyDescent="0.2">
       <c r="A8" s="11"/>
       <c r="B8" s="12"/>
       <c r="C8" s="17"/>
@@ -1001,7 +1001,7 @@
       <c r="P8" s="6"/>
       <c r="Q8" s="6"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="9"/>
       <c r="B9" s="10"/>
       <c r="C9" s="18"/>
@@ -1015,7 +1015,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="11"/>
       <c r="B10" s="12"/>
       <c r="C10" s="17"/>
@@ -1029,7 +1029,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="9"/>
       <c r="B11" s="10"/>
       <c r="C11" s="18"/>
@@ -1043,7 +1043,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="11"/>
       <c r="B12" s="12"/>
       <c r="C12" s="17"/>
@@ -1057,7 +1057,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="9"/>
       <c r="B13" s="10"/>
       <c r="C13" s="18"/>
@@ -1071,7 +1071,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="11"/>
       <c r="B14" s="12"/>
       <c r="C14" s="17"/>
@@ -1085,7 +1085,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="9"/>
       <c r="B15" s="10"/>
       <c r="C15" s="18"/>
@@ -1099,7 +1099,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="11"/>
       <c r="B16" s="12"/>
       <c r="C16" s="17"/>
@@ -1113,7 +1113,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="9"/>
       <c r="B17" s="10"/>
       <c r="C17" s="18"/>
@@ -1127,7 +1127,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="11"/>
       <c r="B18" s="12"/>
       <c r="C18" s="17"/>
@@ -1141,7 +1141,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="9"/>
       <c r="B19" s="10"/>
       <c r="C19" s="18"/>
@@ -1155,7 +1155,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="11"/>
       <c r="B20" s="12"/>
       <c r="C20" s="17"/>
@@ -1169,7 +1169,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="9"/>
       <c r="B21" s="10"/>
       <c r="C21" s="18"/>
@@ -1183,7 +1183,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="11"/>
       <c r="B22" s="12"/>
       <c r="C22" s="17"/>
@@ -1197,7 +1197,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="9"/>
       <c r="B23" s="10"/>
       <c r="C23" s="18"/>
@@ -1211,7 +1211,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="11"/>
       <c r="B24" s="12"/>
       <c r="C24" s="17"/>
@@ -1225,7 +1225,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="9"/>
       <c r="B25" s="10"/>
       <c r="C25" s="18"/>
@@ -1239,7 +1239,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="11"/>
       <c r="B26" s="12"/>
       <c r="C26" s="17"/>
@@ -1253,7 +1253,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="9"/>
       <c r="B27" s="10"/>
       <c r="C27" s="18"/>
@@ -1267,7 +1267,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="11"/>
       <c r="B28" s="12"/>
       <c r="C28" s="17"/>
@@ -1281,7 +1281,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="9"/>
       <c r="B29" s="10"/>
       <c r="C29" s="18"/>
@@ -1295,7 +1295,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="11"/>
       <c r="B30" s="12"/>
       <c r="C30" s="17"/>
@@ -1309,7 +1309,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="9"/>
       <c r="B31" s="10"/>
       <c r="C31" s="18"/>
@@ -1323,7 +1323,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="11"/>
       <c r="B32" s="12"/>
       <c r="C32" s="17"/>
@@ -1337,7 +1337,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="9"/>
       <c r="B33" s="10"/>
       <c r="C33" s="18"/>
@@ -1351,7 +1351,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="11"/>
       <c r="B34" s="12"/>
       <c r="C34" s="17"/>
@@ -1365,7 +1365,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="9"/>
       <c r="B35" s="10"/>
       <c r="C35" s="18"/>
@@ -1379,7 +1379,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="11"/>
       <c r="B36" s="12"/>
       <c r="C36" s="17"/>
@@ -1393,7 +1393,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="9"/>
       <c r="B37" s="10"/>
       <c r="C37" s="18"/>
@@ -1407,7 +1407,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="11"/>
       <c r="B38" s="12"/>
       <c r="C38" s="17"/>
@@ -1421,7 +1421,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="9"/>
       <c r="B39" s="10"/>
       <c r="C39" s="18"/>
@@ -1435,7 +1435,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="11"/>
       <c r="B40" s="12"/>
       <c r="C40" s="17"/>
@@ -1449,7 +1449,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="9"/>
       <c r="B41" s="10"/>
       <c r="C41" s="18"/>
@@ -1463,7 +1463,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="11"/>
       <c r="B42" s="12"/>
       <c r="C42" s="17"/>
@@ -1477,7 +1477,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="9"/>
       <c r="B43" s="10"/>
       <c r="C43" s="18"/>
@@ -1491,7 +1491,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="11"/>
       <c r="B44" s="12"/>
       <c r="C44" s="17"/>
@@ -1505,7 +1505,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="9"/>
       <c r="B45" s="10"/>
       <c r="C45" s="18"/>
@@ -1519,7 +1519,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="11"/>
       <c r="B46" s="12"/>
       <c r="C46" s="17"/>
@@ -1533,7 +1533,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="9"/>
       <c r="B47" s="10"/>
       <c r="C47" s="18"/>
@@ -1547,7 +1547,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="11"/>
       <c r="B48" s="12"/>
       <c r="C48" s="17"/>
@@ -1561,7 +1561,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="9"/>
       <c r="B49" s="10"/>
       <c r="C49" s="18"/>
@@ -1575,7 +1575,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="11"/>
       <c r="B50" s="12"/>
       <c r="C50" s="17"/>
@@ -1589,7 +1589,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="9"/>
       <c r="B51" s="10"/>
       <c r="C51" s="18"/>
@@ -1603,7 +1603,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="7"/>
       <c r="B52" s="8"/>
       <c r="C52" s="19"/>
@@ -1653,43 +1653,43 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.5" customWidth="1"/>
     <col min="2" max="2" width="67" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>4</v>
       </c>
@@ -1708,20 +1708,20 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="42.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E1" s="32" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -1729,27 +1729,27 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ajout de la Typologie T1' dans le tableau des logements
</commit_message>
<xml_diff>
--- a/static/files/logements.xlsx
+++ b/static/files/logements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasoudard/workspace/beta.gouv.fr/apilos/static/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\marjolaine\projets\Beta-Gouv\apilos\static\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{700E8B64-53D6-9E40-A492-0DF20BB04FE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{599EBE63-1DF3-4E59-A6CD-D0D9A225A35C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1400" yWindow="500" windowWidth="27400" windowHeight="16440" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Logements" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Ici quelques explications</t>
   </si>
@@ -148,7 +148,10 @@
     <t>T6 et plus</t>
   </si>
   <si>
-    <t>T1 bis</t>
+    <t>T1'</t>
+  </si>
+  <si>
+    <t>T1bis</t>
   </si>
 </sst>
 </file>
@@ -517,8 +520,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{60458129-C213-8741-80B4-B15A740996D3}" name="type" displayName="type" ref="A1:A8" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3" tableBorderDxfId="2" totalsRowBorderDxfId="1">
-  <autoFilter ref="A1:A8" xr:uid="{60458129-C213-8741-80B4-B15A740996D3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{60458129-C213-8741-80B4-B15A740996D3}" name="type" displayName="type" ref="A1:A9" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3" tableBorderDxfId="2" totalsRowBorderDxfId="1">
+  <autoFilter ref="A1:A9" xr:uid="{60458129-C213-8741-80B4-B15A740996D3}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{68B921AF-0801-1140-A800-5EFE7005DB88}" name="Type de logement" dataDxfId="0"/>
   </tableColumns>
@@ -527,7 +530,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -826,16 +829,16 @@
   <dimension ref="A1:Q52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.6640625" customWidth="1"/>
-    <col min="2" max="9" width="20.83203125" customWidth="1"/>
+    <col min="1" max="1" width="29.625" customWidth="1"/>
+    <col min="2" max="9" width="20.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>19</v>
       </c>
@@ -864,7 +867,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="102" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
         <v>29</v>
       </c>
@@ -879,7 +882,7 @@
       </c>
       <c r="I2" s="37"/>
     </row>
-    <row r="3" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="32" t="s">
         <v>12</v>
       </c>
@@ -907,7 +910,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
       <c r="B4" s="9"/>
       <c r="C4" s="14"/>
@@ -924,7 +927,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="7"/>
       <c r="C5" s="15"/>
@@ -938,7 +941,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="9"/>
       <c r="C6" s="14"/>
@@ -952,7 +955,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="20" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
       <c r="B7" s="7"/>
       <c r="C7" s="15"/>
@@ -974,7 +977,7 @@
       <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
     </row>
-    <row r="8" spans="1:17" ht="20" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A8" s="8"/>
       <c r="B8" s="9"/>
       <c r="C8" s="14"/>
@@ -996,7 +999,7 @@
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="7"/>
       <c r="C9" s="15"/>
@@ -1010,7 +1013,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="9"/>
       <c r="C10" s="14"/>
@@ -1024,7 +1027,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="7"/>
       <c r="C11" s="15"/>
@@ -1038,7 +1041,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="9"/>
       <c r="C12" s="14"/>
@@ -1052,7 +1055,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="7"/>
       <c r="C13" s="15"/>
@@ -1066,7 +1069,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="9"/>
       <c r="C14" s="14"/>
@@ -1080,7 +1083,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="7"/>
       <c r="C15" s="15"/>
@@ -1094,7 +1097,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
       <c r="B16" s="9"/>
       <c r="C16" s="14"/>
@@ -1108,7 +1111,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="7"/>
       <c r="C17" s="15"/>
@@ -1122,7 +1125,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18" s="9"/>
       <c r="C18" s="14"/>
@@ -1136,7 +1139,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="7"/>
       <c r="C19" s="15"/>
@@ -1150,7 +1153,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
       <c r="B20" s="9"/>
       <c r="C20" s="14"/>
@@ -1164,7 +1167,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="7"/>
       <c r="C21" s="15"/>
@@ -1178,7 +1181,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="9"/>
       <c r="C22" s="14"/>
@@ -1192,7 +1195,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="7"/>
       <c r="C23" s="15"/>
@@ -1206,7 +1209,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
       <c r="B24" s="9"/>
       <c r="C24" s="14"/>
@@ -1220,7 +1223,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="7"/>
       <c r="C25" s="15"/>
@@ -1234,7 +1237,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="9"/>
       <c r="C26" s="14"/>
@@ -1248,7 +1251,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="7"/>
       <c r="C27" s="15"/>
@@ -1262,7 +1265,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
       <c r="B28" s="9"/>
       <c r="C28" s="14"/>
@@ -1276,7 +1279,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="7"/>
       <c r="C29" s="15"/>
@@ -1290,7 +1293,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
       <c r="B30" s="9"/>
       <c r="C30" s="14"/>
@@ -1304,7 +1307,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="7"/>
       <c r="C31" s="15"/>
@@ -1318,7 +1321,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
       <c r="B32" s="9"/>
       <c r="C32" s="14"/>
@@ -1332,7 +1335,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
       <c r="B33" s="7"/>
       <c r="C33" s="15"/>
@@ -1346,7 +1349,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
       <c r="B34" s="9"/>
       <c r="C34" s="14"/>
@@ -1360,7 +1363,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
       <c r="B35" s="7"/>
       <c r="C35" s="15"/>
@@ -1374,7 +1377,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
       <c r="B36" s="9"/>
       <c r="C36" s="14"/>
@@ -1388,7 +1391,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
       <c r="B37" s="7"/>
       <c r="C37" s="15"/>
@@ -1402,7 +1405,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="8"/>
       <c r="B38" s="9"/>
       <c r="C38" s="14"/>
@@ -1416,7 +1419,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="7"/>
       <c r="C39" s="15"/>
@@ -1430,7 +1433,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="8"/>
       <c r="B40" s="9"/>
       <c r="C40" s="14"/>
@@ -1444,7 +1447,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="6"/>
       <c r="B41" s="7"/>
       <c r="C41" s="15"/>
@@ -1458,7 +1461,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="8"/>
       <c r="B42" s="9"/>
       <c r="C42" s="14"/>
@@ -1472,7 +1475,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="6"/>
       <c r="B43" s="7"/>
       <c r="C43" s="15"/>
@@ -1486,7 +1489,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="8"/>
       <c r="B44" s="9"/>
       <c r="C44" s="14"/>
@@ -1500,7 +1503,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="6"/>
       <c r="B45" s="7"/>
       <c r="C45" s="15"/>
@@ -1514,7 +1517,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="8"/>
       <c r="B46" s="9"/>
       <c r="C46" s="14"/>
@@ -1528,7 +1531,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="6"/>
       <c r="B47" s="7"/>
       <c r="C47" s="15"/>
@@ -1542,7 +1545,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="8"/>
       <c r="B48" s="9"/>
       <c r="C48" s="14"/>
@@ -1556,7 +1559,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="6"/>
       <c r="B49" s="7"/>
       <c r="C49" s="15"/>
@@ -1570,7 +1573,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="8"/>
       <c r="B50" s="9"/>
       <c r="C50" s="14"/>
@@ -1584,7 +1587,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="6"/>
       <c r="B51" s="7"/>
       <c r="C51" s="15"/>
@@ -1598,7 +1601,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="5"/>
       <c r="B52" s="16"/>
       <c r="C52" s="16"/>
@@ -1632,7 +1635,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{AD40C3CA-AE70-412E-B396-30E460DB0B2E}">
           <x14:formula1>
-            <xm:f>Data!$A$2:$A$8</xm:f>
+            <xm:f>Data!$A$2:$A$9</xm:f>
           </x14:formula1>
           <xm:sqref>B4:B52</xm:sqref>
         </x14:dataValidation>
@@ -1648,43 +1651,43 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.5" customWidth="1"/>
     <col min="2" max="2" width="67" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>4</v>
       </c>
@@ -1697,16 +1700,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4880C39C-0BD9-B447-909B-7F37D33CA805}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
@@ -1714,7 +1719,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -1722,39 +1727,45 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="31"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="31"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="E4" s="31"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>34</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="R38y21+jnu9/6txiWbHyBJZBp+mgqtaPoh0N61YYmEVHWIV+l6U128ETJ6am7UXO1PmMpAO9hLbv8Aby5EG/EQ==" saltValue="ljjfpXf5WSxE5+v64AoXpQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="EFM3dvB/cuEYQctsvfQUkNumpDTn+pz2ZRWwOx0dRgjkbZrkLudh0FyIB0OQEWrHJS+pnGHxfOjUNTVXo90Y0g==" saltValue="pkKJt9fMtr3orPtkO/52zg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
ajout de la Typologie T1' dans le tableau des logements (#1200)
</commit_message>
<xml_diff>
--- a/static/files/logements.xlsx
+++ b/static/files/logements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasoudard/workspace/beta.gouv.fr/apilos/static/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\marjolaine\projets\Beta-Gouv\apilos\static\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{700E8B64-53D6-9E40-A492-0DF20BB04FE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{599EBE63-1DF3-4E59-A6CD-D0D9A225A35C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1400" yWindow="500" windowWidth="27400" windowHeight="16440" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Logements" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Ici quelques explications</t>
   </si>
@@ -148,7 +148,10 @@
     <t>T6 et plus</t>
   </si>
   <si>
-    <t>T1 bis</t>
+    <t>T1'</t>
+  </si>
+  <si>
+    <t>T1bis</t>
   </si>
 </sst>
 </file>
@@ -517,8 +520,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{60458129-C213-8741-80B4-B15A740996D3}" name="type" displayName="type" ref="A1:A8" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3" tableBorderDxfId="2" totalsRowBorderDxfId="1">
-  <autoFilter ref="A1:A8" xr:uid="{60458129-C213-8741-80B4-B15A740996D3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{60458129-C213-8741-80B4-B15A740996D3}" name="type" displayName="type" ref="A1:A9" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3" tableBorderDxfId="2" totalsRowBorderDxfId="1">
+  <autoFilter ref="A1:A9" xr:uid="{60458129-C213-8741-80B4-B15A740996D3}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{68B921AF-0801-1140-A800-5EFE7005DB88}" name="Type de logement" dataDxfId="0"/>
   </tableColumns>
@@ -527,7 +530,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -826,16 +829,16 @@
   <dimension ref="A1:Q52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.6640625" customWidth="1"/>
-    <col min="2" max="9" width="20.83203125" customWidth="1"/>
+    <col min="1" max="1" width="29.625" customWidth="1"/>
+    <col min="2" max="9" width="20.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>19</v>
       </c>
@@ -864,7 +867,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="102" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
         <v>29</v>
       </c>
@@ -879,7 +882,7 @@
       </c>
       <c r="I2" s="37"/>
     </row>
-    <row r="3" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="32" t="s">
         <v>12</v>
       </c>
@@ -907,7 +910,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
       <c r="B4" s="9"/>
       <c r="C4" s="14"/>
@@ -924,7 +927,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="7"/>
       <c r="C5" s="15"/>
@@ -938,7 +941,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="9"/>
       <c r="C6" s="14"/>
@@ -952,7 +955,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="20" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
       <c r="B7" s="7"/>
       <c r="C7" s="15"/>
@@ -974,7 +977,7 @@
       <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
     </row>
-    <row r="8" spans="1:17" ht="20" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A8" s="8"/>
       <c r="B8" s="9"/>
       <c r="C8" s="14"/>
@@ -996,7 +999,7 @@
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="7"/>
       <c r="C9" s="15"/>
@@ -1010,7 +1013,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="9"/>
       <c r="C10" s="14"/>
@@ -1024,7 +1027,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="7"/>
       <c r="C11" s="15"/>
@@ -1038,7 +1041,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="9"/>
       <c r="C12" s="14"/>
@@ -1052,7 +1055,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="7"/>
       <c r="C13" s="15"/>
@@ -1066,7 +1069,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="9"/>
       <c r="C14" s="14"/>
@@ -1080,7 +1083,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="7"/>
       <c r="C15" s="15"/>
@@ -1094,7 +1097,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
       <c r="B16" s="9"/>
       <c r="C16" s="14"/>
@@ -1108,7 +1111,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="7"/>
       <c r="C17" s="15"/>
@@ -1122,7 +1125,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18" s="9"/>
       <c r="C18" s="14"/>
@@ -1136,7 +1139,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="7"/>
       <c r="C19" s="15"/>
@@ -1150,7 +1153,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
       <c r="B20" s="9"/>
       <c r="C20" s="14"/>
@@ -1164,7 +1167,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="7"/>
       <c r="C21" s="15"/>
@@ -1178,7 +1181,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="9"/>
       <c r="C22" s="14"/>
@@ -1192,7 +1195,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="7"/>
       <c r="C23" s="15"/>
@@ -1206,7 +1209,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
       <c r="B24" s="9"/>
       <c r="C24" s="14"/>
@@ -1220,7 +1223,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="7"/>
       <c r="C25" s="15"/>
@@ -1234,7 +1237,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="9"/>
       <c r="C26" s="14"/>
@@ -1248,7 +1251,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="7"/>
       <c r="C27" s="15"/>
@@ -1262,7 +1265,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
       <c r="B28" s="9"/>
       <c r="C28" s="14"/>
@@ -1276,7 +1279,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="7"/>
       <c r="C29" s="15"/>
@@ -1290,7 +1293,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
       <c r="B30" s="9"/>
       <c r="C30" s="14"/>
@@ -1304,7 +1307,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="7"/>
       <c r="C31" s="15"/>
@@ -1318,7 +1321,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
       <c r="B32" s="9"/>
       <c r="C32" s="14"/>
@@ -1332,7 +1335,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
       <c r="B33" s="7"/>
       <c r="C33" s="15"/>
@@ -1346,7 +1349,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
       <c r="B34" s="9"/>
       <c r="C34" s="14"/>
@@ -1360,7 +1363,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
       <c r="B35" s="7"/>
       <c r="C35" s="15"/>
@@ -1374,7 +1377,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
       <c r="B36" s="9"/>
       <c r="C36" s="14"/>
@@ -1388,7 +1391,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
       <c r="B37" s="7"/>
       <c r="C37" s="15"/>
@@ -1402,7 +1405,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="8"/>
       <c r="B38" s="9"/>
       <c r="C38" s="14"/>
@@ -1416,7 +1419,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="7"/>
       <c r="C39" s="15"/>
@@ -1430,7 +1433,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="8"/>
       <c r="B40" s="9"/>
       <c r="C40" s="14"/>
@@ -1444,7 +1447,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="6"/>
       <c r="B41" s="7"/>
       <c r="C41" s="15"/>
@@ -1458,7 +1461,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="8"/>
       <c r="B42" s="9"/>
       <c r="C42" s="14"/>
@@ -1472,7 +1475,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="6"/>
       <c r="B43" s="7"/>
       <c r="C43" s="15"/>
@@ -1486,7 +1489,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="8"/>
       <c r="B44" s="9"/>
       <c r="C44" s="14"/>
@@ -1500,7 +1503,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="6"/>
       <c r="B45" s="7"/>
       <c r="C45" s="15"/>
@@ -1514,7 +1517,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="8"/>
       <c r="B46" s="9"/>
       <c r="C46" s="14"/>
@@ -1528,7 +1531,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="6"/>
       <c r="B47" s="7"/>
       <c r="C47" s="15"/>
@@ -1542,7 +1545,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="8"/>
       <c r="B48" s="9"/>
       <c r="C48" s="14"/>
@@ -1556,7 +1559,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="6"/>
       <c r="B49" s="7"/>
       <c r="C49" s="15"/>
@@ -1570,7 +1573,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="8"/>
       <c r="B50" s="9"/>
       <c r="C50" s="14"/>
@@ -1584,7 +1587,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="6"/>
       <c r="B51" s="7"/>
       <c r="C51" s="15"/>
@@ -1598,7 +1601,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="5"/>
       <c r="B52" s="16"/>
       <c r="C52" s="16"/>
@@ -1632,7 +1635,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{AD40C3CA-AE70-412E-B396-30E460DB0B2E}">
           <x14:formula1>
-            <xm:f>Data!$A$2:$A$8</xm:f>
+            <xm:f>Data!$A$2:$A$9</xm:f>
           </x14:formula1>
           <xm:sqref>B4:B52</xm:sqref>
         </x14:dataValidation>
@@ -1648,43 +1651,43 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.5" customWidth="1"/>
     <col min="2" max="2" width="67" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>4</v>
       </c>
@@ -1697,16 +1700,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4880C39C-0BD9-B447-909B-7F37D33CA805}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
@@ -1714,7 +1719,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -1722,39 +1727,45 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="31"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="31"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="E4" s="31"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>34</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="R38y21+jnu9/6txiWbHyBJZBp+mgqtaPoh0N61YYmEVHWIV+l6U128ETJ6am7UXO1PmMpAO9hLbv8Aby5EG/EQ==" saltValue="ljjfpXf5WSxE5+v64AoXpQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="EFM3dvB/cuEYQctsvfQUkNumpDTn+pz2ZRWwOx0dRgjkbZrkLudh0FyIB0OQEWrHJS+pnGHxfOjUNTVXo90Y0g==" saltValue="pkKJt9fMtr3orPtkO/52zg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
WIP adapter les avenants aux convention mixte
</commit_message>
<xml_diff>
--- a/static/files/logements.xlsx
+++ b/static/files/logements.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayoub.bouchachia\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\production\siap\apilos\static\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B9CB336-2071-427E-BEF6-2274AED39178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F55035CC-1F0E-448F-937F-8571E355743A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16110" yWindow="-18120" windowWidth="29040" windowHeight="17520" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Logements" sheetId="1" r:id="rId1"/>
@@ -71,95 +71,95 @@
     <t>Coefficient propre au logement</t>
   </si>
   <si>
+    <t>(Utilisez votre propre nomenclature, elle doit correspondre à celle indiquée dans l’EDD simplifié, ex : 604, Bâtiment B, étage 4, escalier 3, logement N°604)</t>
+  </si>
+  <si>
+    <t>Par défaut, indiquez un coefficient de 1 si vous n’appliquez pas de pondération particulière)</t>
+  </si>
+  <si>
+    <t>Col 1</t>
+  </si>
+  <si>
+    <t>Col 2</t>
+  </si>
+  <si>
+    <t>Col 3</t>
+  </si>
+  <si>
+    <t>Col 4</t>
+  </si>
+  <si>
+    <t>Col 5</t>
+  </si>
+  <si>
+    <t>Col 6</t>
+  </si>
+  <si>
+    <t>Col 7</t>
+  </si>
+  <si>
+    <t>Col 8</t>
+  </si>
+  <si>
+    <t>Attention : ne pas mettre la ligne Total dans ce tableau</t>
+  </si>
+  <si>
+    <t>elle sera calculée automatiquement lors de l'import des logements</t>
+  </si>
+  <si>
+    <t>Ici quelques explications</t>
+  </si>
+  <si>
+    <t>1. Telechager le modèle (ce fichier)</t>
+  </si>
+  <si>
+    <t>2. Modifier à votre guise le fichier</t>
+  </si>
+  <si>
+    <t>3. Enregistrer vos modifications</t>
+  </si>
+  <si>
+    <t>4. Téléverser le fichier modifié dans l'application</t>
+  </si>
+  <si>
+    <t>5. Vérifier le contenu téléversé dans l'application et enregistrer en cliquant sur le bouton 'Enregistrer et Suivant'</t>
+  </si>
+  <si>
+    <t>Attention, en aucun cas vous ne devez modifier l'entête du tableau des prêts, cela casserait l'import des données</t>
+  </si>
+  <si>
+    <t>Type de logement</t>
+  </si>
+  <si>
+    <t>lignes data</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>T1bis</t>
+  </si>
+  <si>
+    <t>T1'</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>T3</t>
+  </si>
+  <si>
+    <t>T4</t>
+  </si>
+  <si>
+    <t>T5</t>
+  </si>
+  <si>
+    <t>T6 et plus</t>
+  </si>
+  <si>
     <t>Loyer maximum du logement en €
-(col 4 * col 5 * col 6)</t>
-  </si>
-  <si>
-    <t>(Utilisez votre propre nomenclature, elle doit correspondre à celle indiquée dans l’EDD simplifié, ex : 604, Bâtiment B, étage 4, escalier 3, logement N°604)</t>
-  </si>
-  <si>
-    <t>Par défaut, indiquez un coefficient de 1 si vous n’appliquez pas de pondération particulière)</t>
-  </si>
-  <si>
-    <t>Col 1</t>
-  </si>
-  <si>
-    <t>Col 2</t>
-  </si>
-  <si>
-    <t>Col 3</t>
-  </si>
-  <si>
-    <t>Col 4</t>
-  </si>
-  <si>
-    <t>Col 5</t>
-  </si>
-  <si>
-    <t>Col 6</t>
-  </si>
-  <si>
-    <t>Col 7</t>
-  </si>
-  <si>
-    <t>Col 8</t>
-  </si>
-  <si>
-    <t>Attention : ne pas mettre la ligne Total dans ce tableau</t>
-  </si>
-  <si>
-    <t>elle sera calculée automatiquement lors de l'import des logements</t>
-  </si>
-  <si>
-    <t>Ici quelques explications</t>
-  </si>
-  <si>
-    <t>1. Telechager le modèle (ce fichier)</t>
-  </si>
-  <si>
-    <t>2. Modifier à votre guise le fichier</t>
-  </si>
-  <si>
-    <t>3. Enregistrer vos modifications</t>
-  </si>
-  <si>
-    <t>4. Téléverser le fichier modifié dans l'application</t>
-  </si>
-  <si>
-    <t>5. Vérifier le contenu téléversé dans l'application et enregistrer en cliquant sur le bouton 'Enregistrer et Suivant'</t>
-  </si>
-  <si>
-    <t>Attention, en aucun cas vous ne devez modifier l'entête du tableau des prêts, cela casserait l'import des données</t>
-  </si>
-  <si>
-    <t>Type de logement</t>
-  </si>
-  <si>
-    <t>lignes data</t>
-  </si>
-  <si>
-    <t>T1</t>
-  </si>
-  <si>
-    <t>T1bis</t>
-  </si>
-  <si>
-    <t>T1'</t>
-  </si>
-  <si>
-    <t>T2</t>
-  </si>
-  <si>
-    <t>T3</t>
-  </si>
-  <si>
-    <t>T4</t>
-  </si>
-  <si>
-    <t>T5</t>
-  </si>
-  <si>
-    <t>T6 et plus</t>
+(col 5 * col 6 * col 7)</t>
   </si>
 </sst>
 </file>
@@ -840,7 +840,7 @@
   <dimension ref="A1:P52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -880,12 +880,12 @@
         <v>8</v>
       </c>
       <c r="J1" s="37" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="36"/>
       <c r="C2" s="36"/>
@@ -895,39 +895,39 @@
       <c r="G2" s="36"/>
       <c r="H2" s="36"/>
       <c r="I2" s="28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J2" s="38"/>
     </row>
     <row r="3" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="33" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="34"/>
       <c r="C3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="E3" s="34" t="s">
         <v>14</v>
-      </c>
-      <c r="E3" s="34" t="s">
-        <v>15</v>
       </c>
       <c r="F3" s="34"/>
       <c r="G3" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="I3" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="J3" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="K3" s="20" t="s">
         <v>19</v>
-      </c>
-      <c r="K3" s="20" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -942,7 +942,7 @@
       <c r="I4" s="21"/>
       <c r="J4" s="24"/>
       <c r="K4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1720,37 +1720,37 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1772,15 +1772,15 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="29" t="s">
         <v>29</v>
-      </c>
-      <c r="E1" s="29" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E2" s="30">
         <v>4</v>
@@ -1788,39 +1788,39 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E3" s="31"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E4" s="31"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>